<commit_message>
Auto commit - 09171713
</commit_message>
<xml_diff>
--- a/IM/202509_Service_Count_Report.xlsx
+++ b/IM/202509_Service_Count_Report.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AA$257</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AA$258</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
@@ -2688,10 +2688,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB257"/>
+  <dimension ref="A1:AB258"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A257" sqref="A257"/>
+      <selection activeCell="A258" sqref="A258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15461,7 +15461,7 @@
         <v>187</v>
       </c>
       <c r="B189" s="7">
-        <v>2025092052</v>
+        <v>2025092342</v>
       </c>
       <c r="C189" s="7">
         <v>1</v>
@@ -15473,19 +15473,19 @@
         <v>324</v>
       </c>
       <c r="F189" s="7" t="s">
-        <v>176</v>
+        <v>224</v>
       </c>
       <c r="G189" s="7" t="s">
-        <v>359</v>
+        <v>43</v>
       </c>
       <c r="H189" s="7" t="s">
-        <v>514</v>
+        <v>241</v>
       </c>
       <c r="I189" s="7" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="J189" s="7" t="s">
-        <v>516</v>
+        <v>501</v>
       </c>
       <c r="K189" s="7" t="s">
         <v>36</v>
@@ -15497,15 +15497,15 @@
         <v>511</v>
       </c>
       <c r="N189" s="8" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="O189" s="7" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
       <c r="P189" s="7"/>
       <c r="Q189" s="7"/>
       <c r="R189" s="7">
-        <v>58407</v>
+        <v>299068</v>
       </c>
       <c r="S189" s="7"/>
       <c r="T189" s="7"/>
@@ -15513,9 +15513,11 @@
       <c r="V189" s="7"/>
       <c r="W189" s="7"/>
       <c r="X189" s="7"/>
-      <c r="Y189" s="7"/>
+      <c r="Y189" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="Z189" s="8" t="s">
-        <v>518</v>
+        <v>494</v>
       </c>
       <c r="AA189" s="7" t="s">
         <v>40</v>
@@ -15529,7 +15531,7 @@
         <v>188</v>
       </c>
       <c r="B190" s="3">
-        <v>2025092307</v>
+        <v>2025092052</v>
       </c>
       <c r="C190" s="3">
         <v>1</v>
@@ -15541,13 +15543,13 @@
         <v>324</v>
       </c>
       <c r="F190" s="3" t="s">
-        <v>224</v>
+        <v>176</v>
       </c>
       <c r="G190" s="3" t="s">
-        <v>276</v>
+        <v>359</v>
       </c>
       <c r="H190" s="3" t="s">
-        <v>133</v>
+        <v>514</v>
       </c>
       <c r="I190" s="3" t="s">
         <v>515</v>
@@ -15568,12 +15570,12 @@
         <v>517</v>
       </c>
       <c r="O190" s="3" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="P190" s="3"/>
       <c r="Q190" s="3"/>
       <c r="R190" s="3">
-        <v>2041</v>
+        <v>58407</v>
       </c>
       <c r="S190" s="3"/>
       <c r="T190" s="3"/>
@@ -15581,11 +15583,9 @@
       <c r="V190" s="3"/>
       <c r="W190" s="3"/>
       <c r="X190" s="3"/>
-      <c r="Y190" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="Y190" s="3"/>
       <c r="Z190" s="6" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="AA190" s="3" t="s">
         <v>40</v>
@@ -15599,7 +15599,7 @@
         <v>189</v>
       </c>
       <c r="B191" s="7">
-        <v>2025092053</v>
+        <v>2025092307</v>
       </c>
       <c r="C191" s="7">
         <v>1</v>
@@ -15611,16 +15611,16 @@
         <v>324</v>
       </c>
       <c r="F191" s="7" t="s">
-        <v>176</v>
+        <v>224</v>
       </c>
       <c r="G191" s="7" t="s">
-        <v>520</v>
+        <v>276</v>
       </c>
       <c r="H191" s="7" t="s">
-        <v>521</v>
+        <v>133</v>
       </c>
       <c r="I191" s="7" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
       <c r="J191" s="7" t="s">
         <v>516</v>
@@ -15635,15 +15635,15 @@
         <v>511</v>
       </c>
       <c r="N191" s="8" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="O191" s="7" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
       <c r="P191" s="7"/>
       <c r="Q191" s="7"/>
       <c r="R191" s="7">
-        <v>4722</v>
+        <v>2041</v>
       </c>
       <c r="S191" s="7"/>
       <c r="T191" s="7"/>
@@ -15651,9 +15651,11 @@
       <c r="V191" s="7"/>
       <c r="W191" s="7"/>
       <c r="X191" s="7"/>
-      <c r="Y191" s="7"/>
+      <c r="Y191" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="Z191" s="8" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="AA191" s="7" t="s">
         <v>40</v>
@@ -15667,7 +15669,7 @@
         <v>190</v>
       </c>
       <c r="B192" s="3">
-        <v>2025092308</v>
+        <v>2025092053</v>
       </c>
       <c r="C192" s="3">
         <v>1</v>
@@ -15679,13 +15681,13 @@
         <v>324</v>
       </c>
       <c r="F192" s="3" t="s">
-        <v>224</v>
+        <v>176</v>
       </c>
       <c r="G192" s="3" t="s">
-        <v>133</v>
+        <v>520</v>
       </c>
       <c r="H192" s="3" t="s">
-        <v>211</v>
+        <v>521</v>
       </c>
       <c r="I192" s="3" t="s">
         <v>522</v>
@@ -15706,12 +15708,12 @@
         <v>523</v>
       </c>
       <c r="O192" s="3" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="P192" s="3"/>
       <c r="Q192" s="3"/>
       <c r="R192" s="3">
-        <v>23991</v>
+        <v>4722</v>
       </c>
       <c r="S192" s="3"/>
       <c r="T192" s="3"/>
@@ -15719,11 +15721,9 @@
       <c r="V192" s="3"/>
       <c r="W192" s="3"/>
       <c r="X192" s="3"/>
-      <c r="Y192" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="Y192" s="3"/>
       <c r="Z192" s="6" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="AA192" s="3" t="s">
         <v>40</v>
@@ -15737,7 +15737,7 @@
         <v>191</v>
       </c>
       <c r="B193" s="7">
-        <v>2025090337</v>
+        <v>2025092308</v>
       </c>
       <c r="C193" s="7">
         <v>1</v>
@@ -15749,16 +15749,16 @@
         <v>324</v>
       </c>
       <c r="F193" s="7" t="s">
-        <v>190</v>
+        <v>224</v>
       </c>
       <c r="G193" s="7" t="s">
-        <v>342</v>
+        <v>133</v>
       </c>
       <c r="H193" s="7" t="s">
-        <v>96</v>
+        <v>211</v>
       </c>
       <c r="I193" s="7" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="J193" s="7" t="s">
         <v>516</v>
@@ -15767,13 +15767,13 @@
         <v>36</v>
       </c>
       <c r="L193" s="8" t="s">
-        <v>386</v>
+        <v>423</v>
       </c>
       <c r="M193" s="8" t="s">
-        <v>527</v>
+        <v>511</v>
       </c>
       <c r="N193" s="8" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="O193" s="7" t="s">
         <v>39</v>
@@ -15781,29 +15781,33 @@
       <c r="P193" s="7"/>
       <c r="Q193" s="7"/>
       <c r="R193" s="7">
-        <v>48945</v>
-      </c>
-      <c r="S193" s="7" t="s">
-        <v>40</v>
-      </c>
+        <v>23991</v>
+      </c>
+      <c r="S193" s="7"/>
       <c r="T193" s="7"/>
       <c r="U193" s="7"/>
       <c r="V193" s="7"/>
       <c r="W193" s="7"/>
       <c r="X193" s="7"/>
-      <c r="Y193" s="7"/>
+      <c r="Y193" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="Z193" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="AA193" s="7"/>
-      <c r="AB193" s="7"/>
+        <v>525</v>
+      </c>
+      <c r="AA193" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB193" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="194" spans="1:28">
       <c r="A194" s="3">
         <v>192</v>
       </c>
       <c r="B194" s="3">
-        <v>2025090338</v>
+        <v>2025090337</v>
       </c>
       <c r="C194" s="3">
         <v>1</v>
@@ -15842,14 +15846,16 @@
         <v>528</v>
       </c>
       <c r="O194" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P194" s="3"/>
       <c r="Q194" s="3"/>
       <c r="R194" s="3">
         <v>48945</v>
       </c>
-      <c r="S194" s="3"/>
+      <c r="S194" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T194" s="3"/>
       <c r="U194" s="3"/>
       <c r="V194" s="3"/>
@@ -15859,9 +15865,7 @@
       <c r="Z194" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="AA194" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA194" s="3"/>
       <c r="AB194" s="3"/>
     </row>
     <row r="195" spans="1:28">
@@ -15869,7 +15873,7 @@
         <v>193</v>
       </c>
       <c r="B195" s="7">
-        <v>2025090603</v>
+        <v>2025090338</v>
       </c>
       <c r="C195" s="7">
         <v>1</v>
@@ -15881,16 +15885,16 @@
         <v>324</v>
       </c>
       <c r="F195" s="7" t="s">
-        <v>107</v>
+        <v>190</v>
       </c>
       <c r="G195" s="7" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="H195" s="7" t="s">
-        <v>342</v>
+        <v>96</v>
       </c>
       <c r="I195" s="7" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="J195" s="7" t="s">
         <v>516</v>
@@ -15899,25 +15903,23 @@
         <v>36</v>
       </c>
       <c r="L195" s="8" t="s">
-        <v>423</v>
+        <v>386</v>
       </c>
       <c r="M195" s="8" t="s">
-        <v>511</v>
+        <v>527</v>
       </c>
       <c r="N195" s="8" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="O195" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P195" s="7"/>
       <c r="Q195" s="7"/>
       <c r="R195" s="7">
-        <v>13789</v>
-      </c>
-      <c r="S195" s="7" t="s">
-        <v>40</v>
-      </c>
+        <v>48945</v>
+      </c>
+      <c r="S195" s="7"/>
       <c r="T195" s="7"/>
       <c r="U195" s="7"/>
       <c r="V195" s="7"/>
@@ -15927,7 +15929,9 @@
       <c r="Z195" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="AA195" s="7"/>
+      <c r="AA195" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="AB195" s="7"/>
     </row>
     <row r="196" spans="1:28">
@@ -15994,14 +15998,16 @@
       <c r="AA196" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AB196" s="3"/>
+      <c r="AB196" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="197" spans="1:28">
       <c r="A197" s="7">
         <v>195</v>
       </c>
       <c r="B197" s="7">
-        <v>2025092285</v>
+        <v>2025090603</v>
       </c>
       <c r="C197" s="7">
         <v>1</v>
@@ -16013,41 +16019,39 @@
         <v>324</v>
       </c>
       <c r="F197" s="7" t="s">
-        <v>224</v>
+        <v>107</v>
       </c>
       <c r="G197" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="H197" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="H197" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="I197" s="7" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="J197" s="7" t="s">
-        <v>532</v>
+        <v>516</v>
       </c>
       <c r="K197" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L197" s="8" t="s">
-        <v>533</v>
+        <v>423</v>
       </c>
       <c r="M197" s="8" t="s">
-        <v>534</v>
+        <v>511</v>
       </c>
       <c r="N197" s="8" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="O197" s="7" t="s">
         <v>39</v>
       </c>
       <c r="P197" s="7"/>
-      <c r="Q197" s="7">
-        <v>2480</v>
-      </c>
+      <c r="Q197" s="7"/>
       <c r="R197" s="7">
-        <v>172711</v>
+        <v>13789</v>
       </c>
       <c r="S197" s="7" t="s">
         <v>40</v>
@@ -16069,7 +16073,7 @@
         <v>196</v>
       </c>
       <c r="B198" s="3">
-        <v>2025092286</v>
+        <v>2025092285</v>
       </c>
       <c r="C198" s="3">
         <v>1</v>
@@ -16108,7 +16112,7 @@
         <v>535</v>
       </c>
       <c r="O198" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P198" s="3"/>
       <c r="Q198" s="3">
@@ -16117,7 +16121,9 @@
       <c r="R198" s="3">
         <v>172711</v>
       </c>
-      <c r="S198" s="3"/>
+      <c r="S198" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T198" s="3"/>
       <c r="U198" s="3"/>
       <c r="V198" s="3"/>
@@ -16127,9 +16133,7 @@
       <c r="Z198" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="AA198" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA198" s="3"/>
       <c r="AB198" s="3"/>
     </row>
     <row r="199" spans="1:28">
@@ -16137,7 +16141,7 @@
         <v>197</v>
       </c>
       <c r="B199" s="7">
-        <v>2025092287</v>
+        <v>2025092286</v>
       </c>
       <c r="C199" s="7">
         <v>1</v>
@@ -16152,13 +16156,13 @@
         <v>224</v>
       </c>
       <c r="G199" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="H199" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="H199" s="7" t="s">
-        <v>276</v>
-      </c>
       <c r="I199" s="7" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="J199" s="7" t="s">
         <v>532</v>
@@ -16173,21 +16177,19 @@
         <v>534</v>
       </c>
       <c r="N199" s="8" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="O199" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P199" s="7"/>
       <c r="Q199" s="7">
-        <v>8498</v>
+        <v>2480</v>
       </c>
       <c r="R199" s="7">
-        <v>295833</v>
-      </c>
-      <c r="S199" s="7" t="s">
-        <v>40</v>
-      </c>
+        <v>172711</v>
+      </c>
+      <c r="S199" s="7"/>
       <c r="T199" s="7"/>
       <c r="U199" s="7"/>
       <c r="V199" s="7"/>
@@ -16197,7 +16199,9 @@
       <c r="Z199" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="AA199" s="7"/>
+      <c r="AA199" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="AB199" s="7"/>
     </row>
     <row r="200" spans="1:28">
@@ -16205,7 +16209,7 @@
         <v>198</v>
       </c>
       <c r="B200" s="3">
-        <v>2025092288</v>
+        <v>2025092287</v>
       </c>
       <c r="C200" s="3">
         <v>1</v>
@@ -16244,7 +16248,7 @@
         <v>537</v>
       </c>
       <c r="O200" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P200" s="3"/>
       <c r="Q200" s="3">
@@ -16253,7 +16257,9 @@
       <c r="R200" s="3">
         <v>295833</v>
       </c>
-      <c r="S200" s="3"/>
+      <c r="S200" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T200" s="3"/>
       <c r="U200" s="3"/>
       <c r="V200" s="3"/>
@@ -16263,9 +16269,7 @@
       <c r="Z200" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="AA200" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA200" s="3"/>
       <c r="AB200" s="3"/>
     </row>
     <row r="201" spans="1:28">
@@ -16273,7 +16277,7 @@
         <v>199</v>
       </c>
       <c r="B201" s="7">
-        <v>2025090728</v>
+        <v>2025092288</v>
       </c>
       <c r="C201" s="7">
         <v>1</v>
@@ -16285,7 +16289,7 @@
         <v>324</v>
       </c>
       <c r="F201" s="7" t="s">
-        <v>113</v>
+        <v>224</v>
       </c>
       <c r="G201" s="7" t="s">
         <v>96</v>
@@ -16294,34 +16298,34 @@
         <v>276</v>
       </c>
       <c r="I201" s="7" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J201" s="7" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="K201" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L201" s="8" t="s">
-        <v>395</v>
+        <v>533</v>
       </c>
       <c r="M201" s="8" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="N201" s="8" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="O201" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P201" s="7"/>
-      <c r="Q201" s="7"/>
+      <c r="Q201" s="7">
+        <v>8498</v>
+      </c>
       <c r="R201" s="7">
-        <v>25836</v>
-      </c>
-      <c r="S201" s="7" t="s">
-        <v>40</v>
-      </c>
+        <v>295833</v>
+      </c>
+      <c r="S201" s="7"/>
       <c r="T201" s="7"/>
       <c r="U201" s="7"/>
       <c r="V201" s="7"/>
@@ -16334,16 +16338,14 @@
       <c r="AA201" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AB201" s="7">
-        <v>1</v>
-      </c>
+      <c r="AB201" s="7"/>
     </row>
     <row r="202" spans="1:28">
       <c r="A202" s="3">
         <v>200</v>
       </c>
       <c r="B202" s="3">
-        <v>2025090729</v>
+        <v>2025090728</v>
       </c>
       <c r="C202" s="3">
         <v>1</v>
@@ -16382,14 +16384,16 @@
         <v>541</v>
       </c>
       <c r="O202" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P202" s="3"/>
       <c r="Q202" s="3"/>
       <c r="R202" s="3">
         <v>25836</v>
       </c>
-      <c r="S202" s="3"/>
+      <c r="S202" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T202" s="3"/>
       <c r="U202" s="3"/>
       <c r="V202" s="3"/>
@@ -16402,14 +16406,16 @@
       <c r="AA202" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AB202" s="3"/>
+      <c r="AB202" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="203" spans="1:28">
       <c r="A203" s="7">
         <v>201</v>
       </c>
       <c r="B203" s="7">
-        <v>2025091591</v>
+        <v>2025090729</v>
       </c>
       <c r="C203" s="7">
         <v>1</v>
@@ -16421,39 +16427,41 @@
         <v>324</v>
       </c>
       <c r="F203" s="7" t="s">
-        <v>49</v>
+        <v>113</v>
       </c>
       <c r="G203" s="7" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="H203" s="7" t="s">
-        <v>133</v>
+        <v>276</v>
       </c>
       <c r="I203" s="7" t="s">
-        <v>542</v>
-      </c>
-      <c r="J203" s="7"/>
-      <c r="K203" s="7"/>
+        <v>538</v>
+      </c>
+      <c r="J203" s="7" t="s">
+        <v>539</v>
+      </c>
+      <c r="K203" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="L203" s="8" t="s">
-        <v>163</v>
+        <v>395</v>
       </c>
       <c r="M203" s="8" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="N203" s="8" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="O203" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P203" s="7"/>
       <c r="Q203" s="7"/>
       <c r="R203" s="7">
-        <v>0</v>
-      </c>
-      <c r="S203" s="7" t="s">
-        <v>40</v>
-      </c>
+        <v>25836</v>
+      </c>
+      <c r="S203" s="7"/>
       <c r="T203" s="7"/>
       <c r="U203" s="7"/>
       <c r="V203" s="7"/>
@@ -16461,21 +16469,19 @@
       <c r="X203" s="7"/>
       <c r="Y203" s="7"/>
       <c r="Z203" s="8" t="s">
-        <v>184</v>
+        <v>334</v>
       </c>
       <c r="AA203" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AB203" s="7">
-        <v>1</v>
-      </c>
+      <c r="AB203" s="7"/>
     </row>
     <row r="204" spans="1:28">
       <c r="A204" s="3">
         <v>202</v>
       </c>
       <c r="B204" s="3">
-        <v>2025091107</v>
+        <v>2025091591</v>
       </c>
       <c r="C204" s="3">
         <v>1</v>
@@ -16487,41 +16493,39 @@
         <v>324</v>
       </c>
       <c r="F204" s="3" t="s">
-        <v>210</v>
+        <v>49</v>
       </c>
       <c r="G204" s="3" t="s">
-        <v>545</v>
+        <v>33</v>
       </c>
       <c r="H204" s="3" t="s">
-        <v>267</v>
+        <v>133</v>
       </c>
       <c r="I204" s="3" t="s">
-        <v>546</v>
-      </c>
-      <c r="J204" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="K204" s="3" t="s">
-        <v>162</v>
-      </c>
+        <v>542</v>
+      </c>
+      <c r="J204" s="3"/>
+      <c r="K204" s="3"/>
       <c r="L204" s="6" t="s">
         <v>163</v>
       </c>
       <c r="M204" s="6" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="N204" s="6" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="O204" s="3" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
       <c r="P204" s="3"/>
       <c r="Q204" s="3"/>
       <c r="R204" s="3">
         <v>0</v>
       </c>
-      <c r="S204" s="3"/>
+      <c r="S204" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T204" s="3"/>
       <c r="U204" s="3"/>
       <c r="V204" s="3"/>
@@ -16529,7 +16533,7 @@
       <c r="X204" s="3"/>
       <c r="Y204" s="3"/>
       <c r="Z204" s="6" t="s">
-        <v>549</v>
+        <v>184</v>
       </c>
       <c r="AA204" s="3" t="s">
         <v>40</v>
@@ -16546,7 +16550,7 @@
         <v>2025091107</v>
       </c>
       <c r="C205" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D205" s="7" t="s">
         <v>29</v>
@@ -16555,13 +16559,13 @@
         <v>324</v>
       </c>
       <c r="F205" s="7" t="s">
-        <v>49</v>
+        <v>210</v>
       </c>
       <c r="G205" s="7" t="s">
-        <v>96</v>
+        <v>545</v>
       </c>
       <c r="H205" s="7" t="s">
-        <v>550</v>
+        <v>267</v>
       </c>
       <c r="I205" s="7" t="s">
         <v>546</v>
@@ -16597,7 +16601,7 @@
       <c r="X205" s="7"/>
       <c r="Y205" s="7"/>
       <c r="Z205" s="8" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="AA205" s="7" t="s">
         <v>40</v>
@@ -16611,10 +16615,10 @@
         <v>204</v>
       </c>
       <c r="B206" s="3">
-        <v>2025091585</v>
+        <v>2025091107</v>
       </c>
       <c r="C206" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D206" s="3" t="s">
         <v>29</v>
@@ -16626,16 +16630,20 @@
         <v>49</v>
       </c>
       <c r="G206" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H206" s="3" t="s">
         <v>550</v>
-      </c>
-      <c r="H206" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="I206" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="J206" s="3"/>
-      <c r="K206" s="3"/>
+      <c r="J206" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="K206" s="3" t="s">
+        <v>162</v>
+      </c>
       <c r="L206" s="6" t="s">
         <v>163</v>
       </c>
@@ -16646,16 +16654,14 @@
         <v>548</v>
       </c>
       <c r="O206" s="3" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="P206" s="3"/>
       <c r="Q206" s="3"/>
       <c r="R206" s="3">
         <v>0</v>
       </c>
-      <c r="S206" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S206" s="3"/>
       <c r="T206" s="3"/>
       <c r="U206" s="3"/>
       <c r="V206" s="3"/>
@@ -16663,19 +16669,21 @@
       <c r="X206" s="3"/>
       <c r="Y206" s="3"/>
       <c r="Z206" s="6" t="s">
-        <v>184</v>
+        <v>551</v>
       </c>
       <c r="AA206" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AB206" s="3"/>
+      <c r="AB206" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="207" spans="1:28">
       <c r="A207" s="7">
         <v>205</v>
       </c>
       <c r="B207" s="7">
-        <v>2025091610</v>
+        <v>2025091585</v>
       </c>
       <c r="C207" s="7">
         <v>1</v>
@@ -16690,20 +16698,16 @@
         <v>49</v>
       </c>
       <c r="G207" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="H207" s="7" t="s">
-        <v>91</v>
+        <v>33</v>
       </c>
       <c r="I207" s="7" t="s">
         <v>546</v>
       </c>
-      <c r="J207" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="K207" s="7" t="s">
-        <v>162</v>
-      </c>
+      <c r="J207" s="7"/>
+      <c r="K207" s="7"/>
       <c r="L207" s="8" t="s">
         <v>163</v>
       </c>
@@ -16714,14 +16718,16 @@
         <v>548</v>
       </c>
       <c r="O207" s="7" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
       <c r="P207" s="7"/>
       <c r="Q207" s="7"/>
       <c r="R207" s="7">
-        <v>9</v>
-      </c>
-      <c r="S207" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="S207" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T207" s="7"/>
       <c r="U207" s="7"/>
       <c r="V207" s="7"/>
@@ -16729,21 +16735,19 @@
       <c r="X207" s="7"/>
       <c r="Y207" s="7"/>
       <c r="Z207" s="8" t="s">
-        <v>553</v>
+        <v>184</v>
       </c>
       <c r="AA207" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AB207" s="7">
-        <v>1</v>
-      </c>
+      <c r="AB207" s="7"/>
     </row>
     <row r="208" spans="1:28">
       <c r="A208" s="3">
         <v>206</v>
       </c>
       <c r="B208" s="3">
-        <v>2025091593</v>
+        <v>2025091610</v>
       </c>
       <c r="C208" s="3">
         <v>1</v>
@@ -16758,13 +16762,13 @@
         <v>49</v>
       </c>
       <c r="G208" s="3" t="s">
-        <v>168</v>
+        <v>552</v>
       </c>
       <c r="H208" s="3" t="s">
-        <v>197</v>
+        <v>91</v>
       </c>
       <c r="I208" s="3" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="J208" s="3" t="s">
         <v>161</v>
@@ -16776,10 +16780,10 @@
         <v>163</v>
       </c>
       <c r="M208" s="6" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
       <c r="N208" s="6" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="O208" s="3" t="s">
         <v>156</v>
@@ -16787,7 +16791,7 @@
       <c r="P208" s="3"/>
       <c r="Q208" s="3"/>
       <c r="R208" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="S208" s="3"/>
       <c r="T208" s="3"/>
@@ -16797,7 +16801,7 @@
       <c r="X208" s="3"/>
       <c r="Y208" s="3"/>
       <c r="Z208" s="6" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="AA208" s="3" t="s">
         <v>40</v>
@@ -16811,7 +16815,7 @@
         <v>207</v>
       </c>
       <c r="B209" s="7">
-        <v>2025090198</v>
+        <v>2025091593</v>
       </c>
       <c r="C209" s="7">
         <v>1</v>
@@ -16823,39 +16827,41 @@
         <v>324</v>
       </c>
       <c r="F209" s="7" t="s">
-        <v>190</v>
+        <v>49</v>
       </c>
       <c r="G209" s="7" t="s">
-        <v>76</v>
+        <v>168</v>
       </c>
       <c r="H209" s="7" t="s">
-        <v>381</v>
+        <v>197</v>
       </c>
       <c r="I209" s="7" t="s">
-        <v>558</v>
-      </c>
-      <c r="J209" s="7"/>
-      <c r="K209" s="7"/>
+        <v>554</v>
+      </c>
+      <c r="J209" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="K209" s="7" t="s">
+        <v>162</v>
+      </c>
       <c r="L209" s="8" t="s">
         <v>163</v>
       </c>
       <c r="M209" s="8" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="N209" s="8" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="O209" s="7" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="P209" s="7"/>
       <c r="Q209" s="7"/>
       <c r="R209" s="7">
         <v>0</v>
       </c>
-      <c r="S209" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S209" s="7"/>
       <c r="T209" s="7"/>
       <c r="U209" s="7"/>
       <c r="V209" s="7"/>
@@ -16863,7 +16869,7 @@
       <c r="X209" s="7"/>
       <c r="Y209" s="7"/>
       <c r="Z209" s="8" t="s">
-        <v>184</v>
+        <v>557</v>
       </c>
       <c r="AA209" s="7" t="s">
         <v>40</v>
@@ -16877,7 +16883,7 @@
         <v>208</v>
       </c>
       <c r="B210" s="3">
-        <v>2025092032</v>
+        <v>2025090198</v>
       </c>
       <c r="C210" s="3">
         <v>1</v>
@@ -16889,16 +16895,16 @@
         <v>324</v>
       </c>
       <c r="F210" s="3" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="G210" s="3" t="s">
-        <v>133</v>
+        <v>76</v>
       </c>
       <c r="H210" s="3" t="s">
-        <v>241</v>
+        <v>381</v>
       </c>
       <c r="I210" s="3" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="J210" s="3"/>
       <c r="K210" s="3"/>
@@ -16906,10 +16912,10 @@
         <v>163</v>
       </c>
       <c r="M210" s="6" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="N210" s="6" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="O210" s="3" t="s">
         <v>39</v>
@@ -16919,17 +16925,17 @@
       <c r="R210" s="3">
         <v>0</v>
       </c>
-      <c r="S210" s="3"/>
-      <c r="T210" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S210" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T210" s="3"/>
       <c r="U210" s="3"/>
       <c r="V210" s="3"/>
       <c r="W210" s="3"/>
       <c r="X210" s="3"/>
       <c r="Y210" s="3"/>
       <c r="Z210" s="6" t="s">
-        <v>564</v>
+        <v>184</v>
       </c>
       <c r="AA210" s="3" t="s">
         <v>40</v>
@@ -16943,7 +16949,7 @@
         <v>209</v>
       </c>
       <c r="B211" s="7">
-        <v>2025092284</v>
+        <v>2025092032</v>
       </c>
       <c r="C211" s="7">
         <v>1</v>
@@ -16955,13 +16961,13 @@
         <v>324</v>
       </c>
       <c r="F211" s="7" t="s">
-        <v>224</v>
+        <v>176</v>
       </c>
       <c r="G211" s="7" t="s">
-        <v>33</v>
+        <v>133</v>
       </c>
       <c r="H211" s="7" t="s">
-        <v>124</v>
+        <v>241</v>
       </c>
       <c r="I211" s="7" t="s">
         <v>561</v>
@@ -16985,17 +16991,17 @@
       <c r="R211" s="7">
         <v>0</v>
       </c>
-      <c r="S211" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="T211" s="7"/>
+      <c r="S211" s="7"/>
+      <c r="T211" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="U211" s="7"/>
       <c r="V211" s="7"/>
       <c r="W211" s="7"/>
       <c r="X211" s="7"/>
       <c r="Y211" s="7"/>
       <c r="Z211" s="8" t="s">
-        <v>184</v>
+        <v>564</v>
       </c>
       <c r="AA211" s="7" t="s">
         <v>40</v>
@@ -17009,7 +17015,7 @@
         <v>210</v>
       </c>
       <c r="B212" s="3">
-        <v>2025090719</v>
+        <v>2025092284</v>
       </c>
       <c r="C212" s="3">
         <v>1</v>
@@ -17021,41 +17027,39 @@
         <v>324</v>
       </c>
       <c r="F212" s="3" t="s">
-        <v>113</v>
+        <v>224</v>
       </c>
       <c r="G212" s="3" t="s">
-        <v>381</v>
+        <v>33</v>
       </c>
       <c r="H212" s="3" t="s">
-        <v>565</v>
+        <v>124</v>
       </c>
       <c r="I212" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="J212" s="3" t="s">
-        <v>567</v>
-      </c>
-      <c r="K212" s="3" t="s">
-        <v>162</v>
-      </c>
+        <v>561</v>
+      </c>
+      <c r="J212" s="3"/>
+      <c r="K212" s="3"/>
       <c r="L212" s="6" t="s">
         <v>163</v>
       </c>
       <c r="M212" s="6" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="N212" s="6" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="O212" s="3" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
       <c r="P212" s="3"/>
       <c r="Q212" s="3"/>
       <c r="R212" s="3">
         <v>0</v>
       </c>
-      <c r="S212" s="3"/>
+      <c r="S212" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T212" s="3"/>
       <c r="U212" s="3"/>
       <c r="V212" s="3"/>
@@ -17063,7 +17067,7 @@
       <c r="X212" s="3"/>
       <c r="Y212" s="3"/>
       <c r="Z212" s="6" t="s">
-        <v>570</v>
+        <v>184</v>
       </c>
       <c r="AA212" s="3" t="s">
         <v>40</v>
@@ -17077,7 +17081,7 @@
         <v>211</v>
       </c>
       <c r="B213" s="7">
-        <v>2025091568</v>
+        <v>2025090719</v>
       </c>
       <c r="C213" s="7">
         <v>1</v>
@@ -17089,19 +17093,19 @@
         <v>324</v>
       </c>
       <c r="F213" s="7" t="s">
-        <v>49</v>
+        <v>113</v>
       </c>
       <c r="G213" s="7" t="s">
-        <v>211</v>
+        <v>381</v>
       </c>
       <c r="H213" s="7" t="s">
-        <v>76</v>
+        <v>565</v>
       </c>
       <c r="I213" s="7" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="J213" s="7" t="s">
-        <v>161</v>
+        <v>567</v>
       </c>
       <c r="K213" s="7" t="s">
         <v>162</v>
@@ -17110,10 +17114,10 @@
         <v>163</v>
       </c>
       <c r="M213" s="8" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="N213" s="8" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="O213" s="7" t="s">
         <v>156</v>
@@ -17131,7 +17135,7 @@
       <c r="X213" s="7"/>
       <c r="Y213" s="7"/>
       <c r="Z213" s="8" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="AA213" s="7" t="s">
         <v>40</v>
@@ -17145,7 +17149,7 @@
         <v>212</v>
       </c>
       <c r="B214" s="3">
-        <v>2025091070</v>
+        <v>2025091568</v>
       </c>
       <c r="C214" s="3">
         <v>1</v>
@@ -17157,49 +17161,49 @@
         <v>324</v>
       </c>
       <c r="F214" s="3" t="s">
-        <v>275</v>
+        <v>49</v>
       </c>
       <c r="G214" s="3" t="s">
-        <v>96</v>
+        <v>211</v>
       </c>
       <c r="H214" s="3" t="s">
-        <v>276</v>
+        <v>76</v>
       </c>
       <c r="I214" s="3" t="s">
-        <v>575</v>
-      </c>
-      <c r="J214" s="3"/>
-      <c r="K214" s="3"/>
+        <v>571</v>
+      </c>
+      <c r="J214" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="K214" s="3" t="s">
+        <v>162</v>
+      </c>
       <c r="L214" s="6" t="s">
         <v>163</v>
       </c>
       <c r="M214" s="6" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="N214" s="6" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="O214" s="3" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="P214" s="3"/>
       <c r="Q214" s="3"/>
       <c r="R214" s="3">
         <v>0</v>
       </c>
-      <c r="S214" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S214" s="3"/>
       <c r="T214" s="3"/>
       <c r="U214" s="3"/>
       <c r="V214" s="3"/>
       <c r="W214" s="3"/>
       <c r="X214" s="3"/>
-      <c r="Y214" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="Y214" s="3"/>
       <c r="Z214" s="6" t="s">
-        <v>254</v>
+        <v>574</v>
       </c>
       <c r="AA214" s="3" t="s">
         <v>40</v>
@@ -17213,7 +17217,7 @@
         <v>213</v>
       </c>
       <c r="B215" s="7">
-        <v>2025092221</v>
+        <v>2025091070</v>
       </c>
       <c r="C215" s="7">
         <v>1</v>
@@ -17225,23 +17229,19 @@
         <v>324</v>
       </c>
       <c r="F215" s="7" t="s">
-        <v>224</v>
+        <v>275</v>
       </c>
       <c r="G215" s="7" t="s">
-        <v>578</v>
+        <v>96</v>
       </c>
       <c r="H215" s="7" t="s">
-        <v>43</v>
+        <v>276</v>
       </c>
       <c r="I215" s="7" t="s">
         <v>575</v>
       </c>
-      <c r="J215" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="K215" s="7" t="s">
-        <v>162</v>
-      </c>
+      <c r="J215" s="7"/>
+      <c r="K215" s="7"/>
       <c r="L215" s="8" t="s">
         <v>163</v>
       </c>
@@ -17252,22 +17252,26 @@
         <v>577</v>
       </c>
       <c r="O215" s="7" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
       <c r="P215" s="7"/>
       <c r="Q215" s="7"/>
       <c r="R215" s="7">
         <v>0</v>
       </c>
-      <c r="S215" s="7"/>
+      <c r="S215" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T215" s="7"/>
       <c r="U215" s="7"/>
       <c r="V215" s="7"/>
       <c r="W215" s="7"/>
       <c r="X215" s="7"/>
-      <c r="Y215" s="7"/>
+      <c r="Y215" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="Z215" s="8" t="s">
-        <v>579</v>
+        <v>254</v>
       </c>
       <c r="AA215" s="7" t="s">
         <v>40</v>
@@ -17281,7 +17285,7 @@
         <v>214</v>
       </c>
       <c r="B216" s="3">
-        <v>2025090208</v>
+        <v>2025092221</v>
       </c>
       <c r="C216" s="3">
         <v>1</v>
@@ -17293,39 +17297,41 @@
         <v>324</v>
       </c>
       <c r="F216" s="3" t="s">
-        <v>190</v>
+        <v>224</v>
       </c>
       <c r="G216" s="3" t="s">
-        <v>197</v>
+        <v>578</v>
       </c>
       <c r="H216" s="3" t="s">
-        <v>226</v>
+        <v>43</v>
       </c>
       <c r="I216" s="3" t="s">
-        <v>580</v>
-      </c>
-      <c r="J216" s="3"/>
-      <c r="K216" s="3"/>
+        <v>575</v>
+      </c>
+      <c r="J216" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="K216" s="3" t="s">
+        <v>162</v>
+      </c>
       <c r="L216" s="6" t="s">
         <v>163</v>
       </c>
       <c r="M216" s="6" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="N216" s="6" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="O216" s="3" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="P216" s="3"/>
       <c r="Q216" s="3"/>
       <c r="R216" s="3">
         <v>0</v>
       </c>
-      <c r="S216" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S216" s="3"/>
       <c r="T216" s="3"/>
       <c r="U216" s="3"/>
       <c r="V216" s="3"/>
@@ -17333,7 +17339,7 @@
       <c r="X216" s="3"/>
       <c r="Y216" s="3"/>
       <c r="Z216" s="6" t="s">
-        <v>184</v>
+        <v>579</v>
       </c>
       <c r="AA216" s="3" t="s">
         <v>40</v>
@@ -17347,7 +17353,7 @@
         <v>215</v>
       </c>
       <c r="B217" s="7">
-        <v>2025091095</v>
+        <v>2025090208</v>
       </c>
       <c r="C217" s="7">
         <v>1</v>
@@ -17359,16 +17365,16 @@
         <v>324</v>
       </c>
       <c r="F217" s="7" t="s">
-        <v>275</v>
+        <v>190</v>
       </c>
       <c r="G217" s="7" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="H217" s="7" t="s">
-        <v>76</v>
+        <v>226</v>
       </c>
       <c r="I217" s="7" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="J217" s="7"/>
       <c r="K217" s="7"/>
@@ -17376,10 +17382,10 @@
         <v>163</v>
       </c>
       <c r="M217" s="8" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="N217" s="8" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="O217" s="7" t="s">
         <v>39</v>
@@ -17413,7 +17419,7 @@
         <v>216</v>
       </c>
       <c r="B218" s="3">
-        <v>2025091249</v>
+        <v>2025091095</v>
       </c>
       <c r="C218" s="3">
         <v>1</v>
@@ -17425,23 +17431,19 @@
         <v>324</v>
       </c>
       <c r="F218" s="3" t="s">
-        <v>210</v>
+        <v>275</v>
       </c>
       <c r="G218" s="3" t="s">
-        <v>50</v>
+        <v>211</v>
       </c>
       <c r="H218" s="3" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="I218" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="J218" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="K218" s="3" t="s">
-        <v>162</v>
-      </c>
+      <c r="J218" s="3"/>
+      <c r="K218" s="3"/>
       <c r="L218" s="6" t="s">
         <v>163</v>
       </c>
@@ -17452,14 +17454,16 @@
         <v>585</v>
       </c>
       <c r="O218" s="3" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
       <c r="P218" s="3"/>
       <c r="Q218" s="3"/>
       <c r="R218" s="3">
         <v>0</v>
       </c>
-      <c r="S218" s="3"/>
+      <c r="S218" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T218" s="3"/>
       <c r="U218" s="3"/>
       <c r="V218" s="3"/>
@@ -17467,7 +17471,7 @@
       <c r="X218" s="3"/>
       <c r="Y218" s="3"/>
       <c r="Z218" s="6" t="s">
-        <v>586</v>
+        <v>184</v>
       </c>
       <c r="AA218" s="3" t="s">
         <v>40</v>
@@ -17481,7 +17485,7 @@
         <v>217</v>
       </c>
       <c r="B219" s="7">
-        <v>2025091251</v>
+        <v>2025091249</v>
       </c>
       <c r="C219" s="7">
         <v>1</v>
@@ -17496,10 +17500,10 @@
         <v>210</v>
       </c>
       <c r="G219" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H219" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="H219" s="7" t="s">
-        <v>129</v>
       </c>
       <c r="I219" s="7" t="s">
         <v>583</v>
@@ -17535,19 +17539,21 @@
       <c r="X219" s="7"/>
       <c r="Y219" s="7"/>
       <c r="Z219" s="8" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="AA219" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AB219" s="7"/>
+      <c r="AB219" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="220" spans="1:28">
       <c r="A220" s="3">
         <v>218</v>
       </c>
       <c r="B220" s="3">
-        <v>2025091106</v>
+        <v>2025091251</v>
       </c>
       <c r="C220" s="3">
         <v>1</v>
@@ -17559,39 +17565,41 @@
         <v>324</v>
       </c>
       <c r="F220" s="3" t="s">
-        <v>275</v>
+        <v>210</v>
       </c>
       <c r="G220" s="3" t="s">
-        <v>168</v>
+        <v>43</v>
       </c>
       <c r="H220" s="3" t="s">
-        <v>197</v>
+        <v>129</v>
       </c>
       <c r="I220" s="3" t="s">
-        <v>588</v>
-      </c>
-      <c r="J220" s="3"/>
-      <c r="K220" s="3"/>
+        <v>583</v>
+      </c>
+      <c r="J220" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="K220" s="3" t="s">
+        <v>162</v>
+      </c>
       <c r="L220" s="6" t="s">
         <v>163</v>
       </c>
       <c r="M220" s="6" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="N220" s="6" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="O220" s="3" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="P220" s="3"/>
       <c r="Q220" s="3"/>
       <c r="R220" s="3">
         <v>0</v>
       </c>
-      <c r="S220" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S220" s="3"/>
       <c r="T220" s="3"/>
       <c r="U220" s="3"/>
       <c r="V220" s="3"/>
@@ -17599,21 +17607,19 @@
       <c r="X220" s="3"/>
       <c r="Y220" s="3"/>
       <c r="Z220" s="6" t="s">
-        <v>184</v>
+        <v>587</v>
       </c>
       <c r="AA220" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AB220" s="3">
-        <v>1</v>
-      </c>
+      <c r="AB220" s="3"/>
     </row>
     <row r="221" spans="1:28">
       <c r="A221" s="7">
         <v>219</v>
       </c>
       <c r="B221" s="7">
-        <v>2025091113</v>
+        <v>2025091106</v>
       </c>
       <c r="C221" s="7">
         <v>1</v>
@@ -17628,13 +17634,13 @@
         <v>275</v>
       </c>
       <c r="G221" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="H221" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="H221" s="7" t="s">
-        <v>50</v>
-      </c>
       <c r="I221" s="7" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="J221" s="7"/>
       <c r="K221" s="7"/>
@@ -17642,10 +17648,10 @@
         <v>163</v>
       </c>
       <c r="M221" s="8" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="N221" s="8" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="O221" s="7" t="s">
         <v>39</v>
@@ -17679,7 +17685,7 @@
         <v>220</v>
       </c>
       <c r="B222" s="3">
-        <v>2025091076</v>
+        <v>2025091113</v>
       </c>
       <c r="C222" s="3">
         <v>1</v>
@@ -17694,13 +17700,13 @@
         <v>275</v>
       </c>
       <c r="G222" s="3" t="s">
-        <v>276</v>
+        <v>197</v>
       </c>
       <c r="H222" s="3" t="s">
-        <v>133</v>
+        <v>50</v>
       </c>
       <c r="I222" s="3" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="J222" s="3"/>
       <c r="K222" s="3"/>
@@ -17708,10 +17714,10 @@
         <v>163</v>
       </c>
       <c r="M222" s="6" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="N222" s="6" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="O222" s="3" t="s">
         <v>39</v>
@@ -17745,7 +17751,7 @@
         <v>221</v>
       </c>
       <c r="B223" s="7">
-        <v>2025091069</v>
+        <v>2025091076</v>
       </c>
       <c r="C223" s="7">
         <v>1</v>
@@ -17760,13 +17766,13 @@
         <v>275</v>
       </c>
       <c r="G223" s="7" t="s">
-        <v>342</v>
+        <v>276</v>
       </c>
       <c r="H223" s="7" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="I223" s="7" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="J223" s="7"/>
       <c r="K223" s="7"/>
@@ -17774,10 +17780,10 @@
         <v>163</v>
       </c>
       <c r="M223" s="8" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="N223" s="8" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="O223" s="7" t="s">
         <v>39</v>
@@ -17811,7 +17817,7 @@
         <v>222</v>
       </c>
       <c r="B224" s="3">
-        <v>2025090314</v>
+        <v>2025091069</v>
       </c>
       <c r="C224" s="3">
         <v>1</v>
@@ -17823,41 +17829,39 @@
         <v>324</v>
       </c>
       <c r="F224" s="3" t="s">
-        <v>179</v>
+        <v>275</v>
       </c>
       <c r="G224" s="3" t="s">
-        <v>600</v>
+        <v>342</v>
       </c>
       <c r="H224" s="3" t="s">
-        <v>226</v>
+        <v>96</v>
       </c>
       <c r="I224" s="3" t="s">
-        <v>601</v>
-      </c>
-      <c r="J224" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="K224" s="3" t="s">
-        <v>162</v>
-      </c>
+        <v>597</v>
+      </c>
+      <c r="J224" s="3"/>
+      <c r="K224" s="3"/>
       <c r="L224" s="6" t="s">
         <v>163</v>
       </c>
       <c r="M224" s="6" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="N224" s="6" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="O224" s="3" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
       <c r="P224" s="3"/>
       <c r="Q224" s="3"/>
       <c r="R224" s="3">
         <v>0</v>
       </c>
-      <c r="S224" s="3"/>
+      <c r="S224" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T224" s="3"/>
       <c r="U224" s="3"/>
       <c r="V224" s="3"/>
@@ -17865,7 +17869,7 @@
       <c r="X224" s="3"/>
       <c r="Y224" s="3"/>
       <c r="Z224" s="6" t="s">
-        <v>604</v>
+        <v>184</v>
       </c>
       <c r="AA224" s="3" t="s">
         <v>40</v>
@@ -17879,7 +17883,7 @@
         <v>223</v>
       </c>
       <c r="B225" s="7">
-        <v>2025091560</v>
+        <v>2025090314</v>
       </c>
       <c r="C225" s="7">
         <v>1</v>
@@ -17891,10 +17895,10 @@
         <v>324</v>
       </c>
       <c r="F225" s="7" t="s">
-        <v>49</v>
+        <v>179</v>
       </c>
       <c r="G225" s="7" t="s">
-        <v>197</v>
+        <v>600</v>
       </c>
       <c r="H225" s="7" t="s">
         <v>226</v>
@@ -17933,7 +17937,7 @@
       <c r="X225" s="7"/>
       <c r="Y225" s="7"/>
       <c r="Z225" s="8" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AA225" s="7" t="s">
         <v>40</v>
@@ -17947,7 +17951,7 @@
         <v>224</v>
       </c>
       <c r="B226" s="3">
-        <v>2025091469</v>
+        <v>2025091560</v>
       </c>
       <c r="C226" s="3">
         <v>1</v>
@@ -17959,16 +17963,16 @@
         <v>324</v>
       </c>
       <c r="F226" s="3" t="s">
-        <v>210</v>
+        <v>49</v>
       </c>
       <c r="G226" s="3" t="s">
-        <v>381</v>
+        <v>197</v>
       </c>
       <c r="H226" s="3" t="s">
-        <v>352</v>
+        <v>226</v>
       </c>
       <c r="I226" s="3" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="J226" s="3" t="s">
         <v>161</v>
@@ -17980,10 +17984,10 @@
         <v>163</v>
       </c>
       <c r="M226" s="6" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="N226" s="6" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="O226" s="3" t="s">
         <v>156</v>
@@ -18001,7 +18005,7 @@
       <c r="X226" s="3"/>
       <c r="Y226" s="3"/>
       <c r="Z226" s="6" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="AA226" s="3" t="s">
         <v>40</v>
@@ -18015,7 +18019,7 @@
         <v>225</v>
       </c>
       <c r="B227" s="7">
-        <v>2025091603</v>
+        <v>2025091469</v>
       </c>
       <c r="C227" s="7">
         <v>1</v>
@@ -18024,44 +18028,42 @@
         <v>29</v>
       </c>
       <c r="E227" s="7" t="s">
-        <v>610</v>
+        <v>324</v>
       </c>
       <c r="F227" s="7" t="s">
-        <v>49</v>
+        <v>210</v>
       </c>
       <c r="G227" s="7" t="s">
-        <v>611</v>
+        <v>381</v>
       </c>
       <c r="H227" s="7" t="s">
-        <v>612</v>
+        <v>352</v>
       </c>
       <c r="I227" s="7" t="s">
-        <v>613</v>
+        <v>606</v>
       </c>
       <c r="J227" s="7" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="K227" s="7" t="s">
-        <v>36</v>
+        <v>162</v>
       </c>
       <c r="L227" s="8" t="s">
-        <v>614</v>
+        <v>163</v>
       </c>
       <c r="M227" s="8" t="s">
-        <v>615</v>
+        <v>607</v>
       </c>
       <c r="N227" s="8" t="s">
-        <v>410</v>
+        <v>608</v>
       </c>
       <c r="O227" s="7" t="s">
-        <v>42</v>
+        <v>156</v>
       </c>
       <c r="P227" s="7"/>
-      <c r="Q227" s="7">
-        <v>5401</v>
-      </c>
+      <c r="Q227" s="7"/>
       <c r="R227" s="7">
-        <v>61282</v>
+        <v>0</v>
       </c>
       <c r="S227" s="7"/>
       <c r="T227" s="7"/>
@@ -18070,7 +18072,9 @@
       <c r="W227" s="7"/>
       <c r="X227" s="7"/>
       <c r="Y227" s="7"/>
-      <c r="Z227" s="8"/>
+      <c r="Z227" s="8" t="s">
+        <v>609</v>
+      </c>
       <c r="AA227" s="7" t="s">
         <v>40</v>
       </c>
@@ -18083,7 +18087,7 @@
         <v>226</v>
       </c>
       <c r="B228" s="3">
-        <v>2025091604</v>
+        <v>2025091603</v>
       </c>
       <c r="C228" s="3">
         <v>1</v>
@@ -18098,13 +18102,13 @@
         <v>49</v>
       </c>
       <c r="G228" s="3" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="H228" s="3" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="I228" s="3" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="J228" s="3" t="s">
         <v>136</v>
@@ -18126,10 +18130,10 @@
       </c>
       <c r="P228" s="3"/>
       <c r="Q228" s="3">
-        <v>7804</v>
+        <v>5401</v>
       </c>
       <c r="R228" s="3">
-        <v>104403</v>
+        <v>61282</v>
       </c>
       <c r="S228" s="3"/>
       <c r="T228" s="3"/>
@@ -18151,7 +18155,7 @@
         <v>227</v>
       </c>
       <c r="B229" s="7">
-        <v>2025092137</v>
+        <v>2025091604</v>
       </c>
       <c r="C229" s="7">
         <v>1</v>
@@ -18163,48 +18167,50 @@
         <v>610</v>
       </c>
       <c r="F229" s="7" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="G229" s="7" t="s">
-        <v>353</v>
+        <v>616</v>
       </c>
       <c r="H229" s="7" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="I229" s="7" t="s">
-        <v>620</v>
-      </c>
-      <c r="J229" s="7"/>
-      <c r="K229" s="7"/>
+        <v>618</v>
+      </c>
+      <c r="J229" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="K229" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="L229" s="8" t="s">
-        <v>163</v>
+        <v>614</v>
       </c>
       <c r="M229" s="8" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="N229" s="8" t="s">
-        <v>622</v>
+        <v>410</v>
       </c>
       <c r="O229" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P229" s="7"/>
-      <c r="Q229" s="7"/>
+      <c r="Q229" s="7">
+        <v>7804</v>
+      </c>
       <c r="R229" s="7">
-        <v>0</v>
-      </c>
-      <c r="S229" s="7" t="s">
-        <v>40</v>
-      </c>
+        <v>104403</v>
+      </c>
+      <c r="S229" s="7"/>
       <c r="T229" s="7"/>
       <c r="U229" s="7"/>
       <c r="V229" s="7"/>
       <c r="W229" s="7"/>
       <c r="X229" s="7"/>
       <c r="Y229" s="7"/>
-      <c r="Z229" s="8" t="s">
-        <v>184</v>
-      </c>
+      <c r="Z229" s="8"/>
       <c r="AA229" s="7" t="s">
         <v>40</v>
       </c>
@@ -18217,7 +18223,7 @@
         <v>228</v>
       </c>
       <c r="B230" s="3">
-        <v>2025092118</v>
+        <v>2025092137</v>
       </c>
       <c r="C230" s="3">
         <v>1</v>
@@ -18232,13 +18238,13 @@
         <v>31</v>
       </c>
       <c r="G230" s="3" t="s">
-        <v>246</v>
+        <v>353</v>
       </c>
       <c r="H230" s="3" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="I230" s="3" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="J230" s="3"/>
       <c r="K230" s="3"/>
@@ -18246,10 +18252,10 @@
         <v>163</v>
       </c>
       <c r="M230" s="6" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="N230" s="6" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="O230" s="3" t="s">
         <v>39</v>
@@ -18269,7 +18275,7 @@
       <c r="X230" s="3"/>
       <c r="Y230" s="3"/>
       <c r="Z230" s="6" t="s">
-        <v>254</v>
+        <v>184</v>
       </c>
       <c r="AA230" s="3" t="s">
         <v>40</v>
@@ -18283,7 +18289,7 @@
         <v>229</v>
       </c>
       <c r="B231" s="7">
-        <v>2025090356</v>
+        <v>2025092118</v>
       </c>
       <c r="C231" s="7">
         <v>1</v>
@@ -18295,41 +18301,39 @@
         <v>610</v>
       </c>
       <c r="F231" s="7" t="s">
-        <v>179</v>
+        <v>31</v>
       </c>
       <c r="G231" s="7" t="s">
-        <v>627</v>
+        <v>246</v>
       </c>
       <c r="H231" s="7" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="I231" s="7" t="s">
-        <v>629</v>
-      </c>
-      <c r="J231" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="K231" s="7" t="s">
-        <v>162</v>
-      </c>
+        <v>624</v>
+      </c>
+      <c r="J231" s="7"/>
+      <c r="K231" s="7"/>
       <c r="L231" s="8" t="s">
         <v>163</v>
       </c>
       <c r="M231" s="8" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="N231" s="8" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="O231" s="7" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
       <c r="P231" s="7"/>
       <c r="Q231" s="7"/>
       <c r="R231" s="7">
         <v>0</v>
       </c>
-      <c r="S231" s="7"/>
+      <c r="S231" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T231" s="7"/>
       <c r="U231" s="7"/>
       <c r="V231" s="7"/>
@@ -18337,7 +18341,7 @@
       <c r="X231" s="7"/>
       <c r="Y231" s="7"/>
       <c r="Z231" s="8" t="s">
-        <v>632</v>
+        <v>254</v>
       </c>
       <c r="AA231" s="7" t="s">
         <v>40</v>
@@ -18351,7 +18355,7 @@
         <v>230</v>
       </c>
       <c r="B232" s="3">
-        <v>2025092128</v>
+        <v>2025090356</v>
       </c>
       <c r="C232" s="3">
         <v>1</v>
@@ -18363,19 +18367,23 @@
         <v>610</v>
       </c>
       <c r="F232" s="3" t="s">
-        <v>31</v>
+        <v>179</v>
       </c>
       <c r="G232" s="3" t="s">
-        <v>226</v>
+        <v>627</v>
       </c>
       <c r="H232" s="3" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="I232" s="3" t="s">
         <v>629</v>
       </c>
-      <c r="J232" s="3"/>
-      <c r="K232" s="3"/>
+      <c r="J232" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="K232" s="3" t="s">
+        <v>162</v>
+      </c>
       <c r="L232" s="6" t="s">
         <v>163</v>
       </c>
@@ -18386,16 +18394,14 @@
         <v>631</v>
       </c>
       <c r="O232" s="3" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="P232" s="3"/>
       <c r="Q232" s="3"/>
       <c r="R232" s="3">
         <v>0</v>
       </c>
-      <c r="S232" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S232" s="3"/>
       <c r="T232" s="3"/>
       <c r="U232" s="3"/>
       <c r="V232" s="3"/>
@@ -18403,7 +18409,7 @@
       <c r="X232" s="3"/>
       <c r="Y232" s="3"/>
       <c r="Z232" s="6" t="s">
-        <v>184</v>
+        <v>632</v>
       </c>
       <c r="AA232" s="3" t="s">
         <v>40</v>
@@ -18417,7 +18423,7 @@
         <v>231</v>
       </c>
       <c r="B233" s="7">
-        <v>2025090785</v>
+        <v>2025092128</v>
       </c>
       <c r="C233" s="7">
         <v>1</v>
@@ -18429,16 +18435,16 @@
         <v>610</v>
       </c>
       <c r="F233" s="7" t="s">
-        <v>113</v>
+        <v>31</v>
       </c>
       <c r="G233" s="7" t="s">
-        <v>634</v>
+        <v>226</v>
       </c>
       <c r="H233" s="7" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="I233" s="7" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
       <c r="J233" s="7"/>
       <c r="K233" s="7"/>
@@ -18446,10 +18452,10 @@
         <v>163</v>
       </c>
       <c r="M233" s="8" t="s">
-        <v>637</v>
+        <v>630</v>
       </c>
       <c r="N233" s="8" t="s">
-        <v>638</v>
+        <v>631</v>
       </c>
       <c r="O233" s="7" t="s">
         <v>39</v>
@@ -18483,7 +18489,7 @@
         <v>232</v>
       </c>
       <c r="B234" s="3">
-        <v>2025090801</v>
+        <v>2025090785</v>
       </c>
       <c r="C234" s="3">
         <v>1</v>
@@ -18498,13 +18504,13 @@
         <v>113</v>
       </c>
       <c r="G234" s="3" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="H234" s="3" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="I234" s="3" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="J234" s="3"/>
       <c r="K234" s="3"/>
@@ -18512,10 +18518,10 @@
         <v>163</v>
       </c>
       <c r="M234" s="6" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="N234" s="6" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="O234" s="3" t="s">
         <v>39</v>
@@ -18549,7 +18555,7 @@
         <v>233</v>
       </c>
       <c r="B235" s="7">
-        <v>2025092117</v>
+        <v>2025090801</v>
       </c>
       <c r="C235" s="7">
         <v>1</v>
@@ -18561,16 +18567,16 @@
         <v>610</v>
       </c>
       <c r="F235" s="7" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="G235" s="7" t="s">
-        <v>245</v>
+        <v>639</v>
       </c>
       <c r="H235" s="7" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="I235" s="7" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="J235" s="7"/>
       <c r="K235" s="7"/>
@@ -18578,10 +18584,10 @@
         <v>163</v>
       </c>
       <c r="M235" s="8" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="N235" s="8" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="O235" s="7" t="s">
         <v>39</v>
@@ -18615,7 +18621,7 @@
         <v>234</v>
       </c>
       <c r="B236" s="3">
-        <v>2025092124</v>
+        <v>2025092117</v>
       </c>
       <c r="C236" s="3">
         <v>1</v>
@@ -18630,13 +18636,13 @@
         <v>31</v>
       </c>
       <c r="G236" s="3" t="s">
-        <v>648</v>
+        <v>245</v>
       </c>
       <c r="H236" s="3" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="I236" s="3" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="J236" s="3"/>
       <c r="K236" s="3"/>
@@ -18644,10 +18650,10 @@
         <v>163</v>
       </c>
       <c r="M236" s="6" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="N236" s="6" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="O236" s="3" t="s">
         <v>39</v>
@@ -18681,7 +18687,7 @@
         <v>235</v>
       </c>
       <c r="B237" s="7">
-        <v>2025090382</v>
+        <v>2025092124</v>
       </c>
       <c r="C237" s="7">
         <v>1</v>
@@ -18693,16 +18699,16 @@
         <v>610</v>
       </c>
       <c r="F237" s="7" t="s">
-        <v>179</v>
+        <v>31</v>
       </c>
       <c r="G237" s="7" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="H237" s="7" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="I237" s="7" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="J237" s="7"/>
       <c r="K237" s="7"/>
@@ -18710,10 +18716,10 @@
         <v>163</v>
       </c>
       <c r="M237" s="8" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="N237" s="8" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="O237" s="7" t="s">
         <v>39</v>
@@ -18747,7 +18753,7 @@
         <v>236</v>
       </c>
       <c r="B238" s="3">
-        <v>2025090307</v>
+        <v>2025090382</v>
       </c>
       <c r="C238" s="3">
         <v>1</v>
@@ -18765,17 +18771,13 @@
         <v>653</v>
       </c>
       <c r="H238" s="3" t="s">
-        <v>550</v>
+        <v>654</v>
       </c>
       <c r="I238" s="3" t="s">
         <v>655</v>
       </c>
-      <c r="J238" s="3" t="s">
-        <v>567</v>
-      </c>
-      <c r="K238" s="3" t="s">
-        <v>162</v>
-      </c>
+      <c r="J238" s="3"/>
+      <c r="K238" s="3"/>
       <c r="L238" s="6" t="s">
         <v>163</v>
       </c>
@@ -18786,14 +18788,16 @@
         <v>657</v>
       </c>
       <c r="O238" s="3" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
       <c r="P238" s="3"/>
       <c r="Q238" s="3"/>
       <c r="R238" s="3">
         <v>0</v>
       </c>
-      <c r="S238" s="3"/>
+      <c r="S238" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T238" s="3"/>
       <c r="U238" s="3"/>
       <c r="V238" s="3"/>
@@ -18801,19 +18805,21 @@
       <c r="X238" s="3"/>
       <c r="Y238" s="3"/>
       <c r="Z238" s="6" t="s">
-        <v>658</v>
+        <v>184</v>
       </c>
       <c r="AA238" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AB238" s="3"/>
+      <c r="AB238" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="239" spans="1:28">
       <c r="A239" s="7">
         <v>237</v>
       </c>
       <c r="B239" s="7">
-        <v>2025090012</v>
+        <v>2025090307</v>
       </c>
       <c r="C239" s="7">
         <v>1</v>
@@ -18828,16 +18834,16 @@
         <v>179</v>
       </c>
       <c r="G239" s="7" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="H239" s="7" t="s">
-        <v>660</v>
+        <v>550</v>
       </c>
       <c r="I239" s="7" t="s">
         <v>655</v>
       </c>
       <c r="J239" s="7" t="s">
-        <v>161</v>
+        <v>567</v>
       </c>
       <c r="K239" s="7" t="s">
         <v>162</v>
@@ -18867,7 +18873,7 @@
       <c r="X239" s="7"/>
       <c r="Y239" s="7"/>
       <c r="Z239" s="8" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="AA239" s="7" t="s">
         <v>40</v>
@@ -18879,7 +18885,7 @@
         <v>238</v>
       </c>
       <c r="B240" s="3">
-        <v>2025090712</v>
+        <v>2025090012</v>
       </c>
       <c r="C240" s="3">
         <v>1</v>
@@ -18891,16 +18897,16 @@
         <v>610</v>
       </c>
       <c r="F240" s="3" t="s">
-        <v>113</v>
+        <v>179</v>
       </c>
       <c r="G240" s="3" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="H240" s="3" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="I240" s="3" t="s">
-        <v>664</v>
+        <v>655</v>
       </c>
       <c r="J240" s="3" t="s">
         <v>161</v>
@@ -18912,10 +18918,10 @@
         <v>163</v>
       </c>
       <c r="M240" s="6" t="s">
-        <v>665</v>
+        <v>656</v>
       </c>
       <c r="N240" s="6" t="s">
-        <v>666</v>
+        <v>657</v>
       </c>
       <c r="O240" s="3" t="s">
         <v>156</v>
@@ -18933,21 +18939,19 @@
       <c r="X240" s="3"/>
       <c r="Y240" s="3"/>
       <c r="Z240" s="6" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="AA240" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AB240" s="3">
-        <v>1</v>
-      </c>
+      <c r="AB240" s="3"/>
     </row>
     <row r="241" spans="1:28">
       <c r="A241" s="7">
         <v>239</v>
       </c>
       <c r="B241" s="7">
-        <v>2025090821</v>
+        <v>2025090712</v>
       </c>
       <c r="C241" s="7">
         <v>1</v>
@@ -18970,8 +18974,12 @@
       <c r="I241" s="7" t="s">
         <v>664</v>
       </c>
-      <c r="J241" s="7"/>
-      <c r="K241" s="7"/>
+      <c r="J241" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="K241" s="7" t="s">
+        <v>162</v>
+      </c>
       <c r="L241" s="8" t="s">
         <v>163</v>
       </c>
@@ -18982,36 +18990,36 @@
         <v>666</v>
       </c>
       <c r="O241" s="7" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="P241" s="7"/>
       <c r="Q241" s="7"/>
       <c r="R241" s="7">
         <v>0</v>
       </c>
-      <c r="S241" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S241" s="7"/>
       <c r="T241" s="7"/>
       <c r="U241" s="7"/>
       <c r="V241" s="7"/>
       <c r="W241" s="7"/>
       <c r="X241" s="7"/>
-      <c r="Y241" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="Y241" s="7"/>
       <c r="Z241" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="AA241" s="7"/>
-      <c r="AB241" s="7"/>
+        <v>667</v>
+      </c>
+      <c r="AA241" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB241" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="242" spans="1:28">
       <c r="A242" s="3">
         <v>240</v>
       </c>
       <c r="B242" s="3">
-        <v>2025090957</v>
+        <v>2025090821</v>
       </c>
       <c r="C242" s="3">
         <v>1</v>
@@ -19023,23 +19031,19 @@
         <v>610</v>
       </c>
       <c r="F242" s="3" t="s">
-        <v>275</v>
+        <v>113</v>
       </c>
       <c r="G242" s="3" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="H242" s="3" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="I242" s="3" t="s">
         <v>664</v>
       </c>
-      <c r="J242" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="K242" s="3" t="s">
-        <v>162</v>
-      </c>
+      <c r="J242" s="3"/>
+      <c r="K242" s="3"/>
       <c r="L242" s="6" t="s">
         <v>163</v>
       </c>
@@ -19050,36 +19054,36 @@
         <v>666</v>
       </c>
       <c r="O242" s="3" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
       <c r="P242" s="3"/>
       <c r="Q242" s="3"/>
       <c r="R242" s="3">
         <v>0</v>
       </c>
-      <c r="S242" s="3"/>
+      <c r="S242" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T242" s="3"/>
       <c r="U242" s="3"/>
       <c r="V242" s="3"/>
       <c r="W242" s="3"/>
       <c r="X242" s="3"/>
-      <c r="Y242" s="3"/>
+      <c r="Y242" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="Z242" s="6" t="s">
-        <v>632</v>
-      </c>
-      <c r="AA242" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB242" s="3">
-        <v>1</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="AA242" s="3"/>
+      <c r="AB242" s="3"/>
     </row>
     <row r="243" spans="1:28">
       <c r="A243" s="7">
         <v>241</v>
       </c>
       <c r="B243" s="7">
-        <v>2025090555</v>
+        <v>2025090957</v>
       </c>
       <c r="C243" s="7">
         <v>1</v>
@@ -19091,16 +19095,16 @@
         <v>610</v>
       </c>
       <c r="F243" s="7" t="s">
-        <v>113</v>
+        <v>275</v>
       </c>
       <c r="G243" s="7" t="s">
-        <v>381</v>
+        <v>668</v>
       </c>
       <c r="H243" s="7" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I243" s="7" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
       <c r="J243" s="7" t="s">
         <v>161</v>
@@ -19112,10 +19116,10 @@
         <v>163</v>
       </c>
       <c r="M243" s="8" t="s">
-        <v>672</v>
+        <v>665</v>
       </c>
       <c r="N243" s="8" t="s">
-        <v>673</v>
+        <v>666</v>
       </c>
       <c r="O243" s="7" t="s">
         <v>156</v>
@@ -19133,7 +19137,7 @@
       <c r="X243" s="7"/>
       <c r="Y243" s="7"/>
       <c r="Z243" s="8" t="s">
-        <v>674</v>
+        <v>632</v>
       </c>
       <c r="AA243" s="7" t="s">
         <v>40</v>
@@ -19147,7 +19151,7 @@
         <v>242</v>
       </c>
       <c r="B244" s="3">
-        <v>2025090857</v>
+        <v>2025090555</v>
       </c>
       <c r="C244" s="3">
         <v>1</v>
@@ -19159,13 +19163,13 @@
         <v>610</v>
       </c>
       <c r="F244" s="3" t="s">
-        <v>149</v>
+        <v>113</v>
       </c>
       <c r="G244" s="3" t="s">
-        <v>675</v>
+        <v>381</v>
       </c>
       <c r="H244" s="3" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
       <c r="I244" s="3" t="s">
         <v>671</v>
@@ -19201,7 +19205,7 @@
       <c r="X244" s="3"/>
       <c r="Y244" s="3"/>
       <c r="Z244" s="6" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="AA244" s="3" t="s">
         <v>40</v>
@@ -19215,7 +19219,7 @@
         <v>243</v>
       </c>
       <c r="B245" s="7">
-        <v>2025090805</v>
+        <v>2025090857</v>
       </c>
       <c r="C245" s="7">
         <v>1</v>
@@ -19227,39 +19231,41 @@
         <v>610</v>
       </c>
       <c r="F245" s="7" t="s">
-        <v>113</v>
+        <v>149</v>
       </c>
       <c r="G245" s="7" t="s">
-        <v>320</v>
+        <v>675</v>
       </c>
       <c r="H245" s="7" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="I245" s="7" t="s">
-        <v>679</v>
-      </c>
-      <c r="J245" s="7"/>
-      <c r="K245" s="7"/>
+        <v>671</v>
+      </c>
+      <c r="J245" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="K245" s="7" t="s">
+        <v>162</v>
+      </c>
       <c r="L245" s="8" t="s">
         <v>163</v>
       </c>
       <c r="M245" s="8" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="N245" s="8" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="O245" s="7" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="P245" s="7"/>
       <c r="Q245" s="7"/>
       <c r="R245" s="7">
         <v>0</v>
       </c>
-      <c r="S245" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S245" s="7"/>
       <c r="T245" s="7"/>
       <c r="U245" s="7"/>
       <c r="V245" s="7"/>
@@ -19267,7 +19273,7 @@
       <c r="X245" s="7"/>
       <c r="Y245" s="7"/>
       <c r="Z245" s="8" t="s">
-        <v>184</v>
+        <v>677</v>
       </c>
       <c r="AA245" s="7" t="s">
         <v>40</v>
@@ -19281,7 +19287,7 @@
         <v>244</v>
       </c>
       <c r="B246" s="3">
-        <v>2025092145</v>
+        <v>2025090805</v>
       </c>
       <c r="C246" s="3">
         <v>1</v>
@@ -19293,41 +19299,39 @@
         <v>610</v>
       </c>
       <c r="F246" s="3" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="G246" s="3" t="s">
-        <v>682</v>
+        <v>320</v>
       </c>
       <c r="H246" s="3" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="I246" s="3" t="s">
-        <v>684</v>
-      </c>
-      <c r="J246" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="K246" s="3" t="s">
-        <v>162</v>
-      </c>
+        <v>679</v>
+      </c>
+      <c r="J246" s="3"/>
+      <c r="K246" s="3"/>
       <c r="L246" s="6" t="s">
         <v>163</v>
       </c>
       <c r="M246" s="6" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="N246" s="6" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="O246" s="3" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
       <c r="P246" s="3"/>
       <c r="Q246" s="3"/>
       <c r="R246" s="3">
         <v>0</v>
       </c>
-      <c r="S246" s="3"/>
+      <c r="S246" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T246" s="3"/>
       <c r="U246" s="3"/>
       <c r="V246" s="3"/>
@@ -19335,7 +19339,7 @@
       <c r="X246" s="3"/>
       <c r="Y246" s="3"/>
       <c r="Z246" s="6" t="s">
-        <v>687</v>
+        <v>184</v>
       </c>
       <c r="AA246" s="3" t="s">
         <v>40</v>
@@ -19349,7 +19353,7 @@
         <v>245</v>
       </c>
       <c r="B247" s="7">
-        <v>2025091105</v>
+        <v>2025092145</v>
       </c>
       <c r="C247" s="7">
         <v>1</v>
@@ -19361,16 +19365,16 @@
         <v>610</v>
       </c>
       <c r="F247" s="7" t="s">
-        <v>275</v>
+        <v>31</v>
       </c>
       <c r="G247" s="7" t="s">
-        <v>688</v>
+        <v>682</v>
       </c>
       <c r="H247" s="7" t="s">
-        <v>689</v>
+        <v>683</v>
       </c>
       <c r="I247" s="7" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="J247" s="7" t="s">
         <v>161</v>
@@ -19382,10 +19386,10 @@
         <v>163</v>
       </c>
       <c r="M247" s="8" t="s">
-        <v>691</v>
+        <v>685</v>
       </c>
       <c r="N247" s="8" t="s">
-        <v>692</v>
+        <v>686</v>
       </c>
       <c r="O247" s="7" t="s">
         <v>156</v>
@@ -19403,7 +19407,7 @@
       <c r="X247" s="7"/>
       <c r="Y247" s="7"/>
       <c r="Z247" s="8" t="s">
-        <v>661</v>
+        <v>687</v>
       </c>
       <c r="AA247" s="7" t="s">
         <v>40</v>
@@ -19417,7 +19421,7 @@
         <v>246</v>
       </c>
       <c r="B248" s="3">
-        <v>2025091130</v>
+        <v>2025091105</v>
       </c>
       <c r="C248" s="3">
         <v>1</v>
@@ -19432,16 +19436,16 @@
         <v>275</v>
       </c>
       <c r="G248" s="3" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="H248" s="3" t="s">
-        <v>261</v>
+        <v>689</v>
       </c>
       <c r="I248" s="3" t="s">
         <v>690</v>
       </c>
       <c r="J248" s="3" t="s">
-        <v>567</v>
+        <v>161</v>
       </c>
       <c r="K248" s="3" t="s">
         <v>162</v>
@@ -19471,19 +19475,21 @@
       <c r="X248" s="3"/>
       <c r="Y248" s="3"/>
       <c r="Z248" s="6" t="s">
-        <v>694</v>
+        <v>661</v>
       </c>
       <c r="AA248" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AB248" s="3"/>
+      <c r="AB248" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="249" spans="1:28">
       <c r="A249" s="7">
         <v>247</v>
       </c>
       <c r="B249" s="7">
-        <v>2025090814</v>
+        <v>2025091130</v>
       </c>
       <c r="C249" s="7">
         <v>1</v>
@@ -19495,39 +19501,41 @@
         <v>610</v>
       </c>
       <c r="F249" s="7" t="s">
-        <v>113</v>
+        <v>275</v>
       </c>
       <c r="G249" s="7" t="s">
-        <v>51</v>
+        <v>693</v>
       </c>
       <c r="H249" s="7" t="s">
-        <v>695</v>
+        <v>261</v>
       </c>
       <c r="I249" s="7" t="s">
-        <v>696</v>
-      </c>
-      <c r="J249" s="7"/>
-      <c r="K249" s="7"/>
+        <v>690</v>
+      </c>
+      <c r="J249" s="7" t="s">
+        <v>567</v>
+      </c>
+      <c r="K249" s="7" t="s">
+        <v>162</v>
+      </c>
       <c r="L249" s="8" t="s">
         <v>163</v>
       </c>
       <c r="M249" s="8" t="s">
-        <v>697</v>
+        <v>691</v>
       </c>
       <c r="N249" s="8" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
       <c r="O249" s="7" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="P249" s="7"/>
       <c r="Q249" s="7"/>
       <c r="R249" s="7">
         <v>0</v>
       </c>
-      <c r="S249" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S249" s="7"/>
       <c r="T249" s="7"/>
       <c r="U249" s="7"/>
       <c r="V249" s="7"/>
@@ -19535,21 +19543,19 @@
       <c r="X249" s="7"/>
       <c r="Y249" s="7"/>
       <c r="Z249" s="8" t="s">
-        <v>184</v>
+        <v>694</v>
       </c>
       <c r="AA249" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AB249" s="7">
-        <v>1</v>
-      </c>
+      <c r="AB249" s="7"/>
     </row>
     <row r="250" spans="1:28">
       <c r="A250" s="3">
         <v>248</v>
       </c>
       <c r="B250" s="3">
-        <v>2025091612</v>
+        <v>2025090814</v>
       </c>
       <c r="C250" s="3">
         <v>1</v>
@@ -19561,23 +19567,19 @@
         <v>610</v>
       </c>
       <c r="F250" s="3" t="s">
-        <v>167</v>
+        <v>113</v>
       </c>
       <c r="G250" s="3" t="s">
-        <v>640</v>
+        <v>51</v>
       </c>
       <c r="H250" s="3" t="s">
-        <v>320</v>
+        <v>695</v>
       </c>
       <c r="I250" s="3" t="s">
         <v>696</v>
       </c>
-      <c r="J250" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="K250" s="3" t="s">
-        <v>162</v>
-      </c>
+      <c r="J250" s="3"/>
+      <c r="K250" s="3"/>
       <c r="L250" s="6" t="s">
         <v>163</v>
       </c>
@@ -19588,14 +19590,16 @@
         <v>698</v>
       </c>
       <c r="O250" s="3" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
       <c r="P250" s="3"/>
       <c r="Q250" s="3"/>
       <c r="R250" s="3">
         <v>0</v>
       </c>
-      <c r="S250" s="3"/>
+      <c r="S250" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T250" s="3"/>
       <c r="U250" s="3"/>
       <c r="V250" s="3"/>
@@ -19603,7 +19607,7 @@
       <c r="X250" s="3"/>
       <c r="Y250" s="3"/>
       <c r="Z250" s="6" t="s">
-        <v>699</v>
+        <v>184</v>
       </c>
       <c r="AA250" s="3" t="s">
         <v>40</v>
@@ -19617,7 +19621,7 @@
         <v>249</v>
       </c>
       <c r="B251" s="7">
-        <v>2025091812</v>
+        <v>2025091612</v>
       </c>
       <c r="C251" s="7">
         <v>1</v>
@@ -19635,7 +19639,7 @@
         <v>640</v>
       </c>
       <c r="H251" s="7" t="s">
-        <v>700</v>
+        <v>320</v>
       </c>
       <c r="I251" s="7" t="s">
         <v>696</v>
@@ -19671,19 +19675,21 @@
       <c r="X251" s="7"/>
       <c r="Y251" s="7"/>
       <c r="Z251" s="8" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="AA251" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AB251" s="7"/>
+      <c r="AB251" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="252" spans="1:28">
       <c r="A252" s="3">
         <v>250</v>
       </c>
       <c r="B252" s="3">
-        <v>2025091738</v>
+        <v>2025091812</v>
       </c>
       <c r="C252" s="3">
         <v>1</v>
@@ -19698,10 +19704,10 @@
         <v>167</v>
       </c>
       <c r="G252" s="3" t="s">
-        <v>702</v>
+        <v>640</v>
       </c>
       <c r="H252" s="3" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="I252" s="3" t="s">
         <v>696</v>
@@ -19737,7 +19743,7 @@
       <c r="X252" s="3"/>
       <c r="Y252" s="3"/>
       <c r="Z252" s="6" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="AA252" s="3" t="s">
         <v>40</v>
@@ -19749,7 +19755,7 @@
         <v>251</v>
       </c>
       <c r="B253" s="7">
-        <v>2025090963</v>
+        <v>2025091738</v>
       </c>
       <c r="C253" s="7">
         <v>1</v>
@@ -19761,16 +19767,16 @@
         <v>610</v>
       </c>
       <c r="F253" s="7" t="s">
-        <v>275</v>
+        <v>167</v>
       </c>
       <c r="G253" s="7" t="s">
-        <v>69</v>
+        <v>702</v>
       </c>
       <c r="H253" s="7" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="I253" s="7" t="s">
-        <v>706</v>
+        <v>696</v>
       </c>
       <c r="J253" s="7" t="s">
         <v>161</v>
@@ -19782,10 +19788,10 @@
         <v>163</v>
       </c>
       <c r="M253" s="8" t="s">
-        <v>707</v>
+        <v>697</v>
       </c>
       <c r="N253" s="8" t="s">
-        <v>708</v>
+        <v>698</v>
       </c>
       <c r="O253" s="7" t="s">
         <v>156</v>
@@ -19803,21 +19809,19 @@
       <c r="X253" s="7"/>
       <c r="Y253" s="7"/>
       <c r="Z253" s="8" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="AA253" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AB253" s="7">
-        <v>1</v>
-      </c>
+      <c r="AB253" s="7"/>
     </row>
     <row r="254" spans="1:28">
       <c r="A254" s="3">
         <v>252</v>
       </c>
       <c r="B254" s="3">
-        <v>2025090797</v>
+        <v>2025090963</v>
       </c>
       <c r="C254" s="3">
         <v>1</v>
@@ -19829,39 +19833,41 @@
         <v>610</v>
       </c>
       <c r="F254" s="3" t="s">
-        <v>113</v>
+        <v>275</v>
       </c>
       <c r="G254" s="3" t="s">
-        <v>353</v>
+        <v>69</v>
       </c>
       <c r="H254" s="3" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="I254" s="3" t="s">
-        <v>711</v>
-      </c>
-      <c r="J254" s="3"/>
-      <c r="K254" s="3"/>
+        <v>706</v>
+      </c>
+      <c r="J254" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="K254" s="3" t="s">
+        <v>162</v>
+      </c>
       <c r="L254" s="6" t="s">
         <v>163</v>
       </c>
       <c r="M254" s="6" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="N254" s="6" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
       <c r="O254" s="3" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="P254" s="3"/>
       <c r="Q254" s="3"/>
       <c r="R254" s="3">
         <v>0</v>
       </c>
-      <c r="S254" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S254" s="3"/>
       <c r="T254" s="3"/>
       <c r="U254" s="3"/>
       <c r="V254" s="3"/>
@@ -19869,7 +19875,7 @@
       <c r="X254" s="3"/>
       <c r="Y254" s="3"/>
       <c r="Z254" s="6" t="s">
-        <v>184</v>
+        <v>709</v>
       </c>
       <c r="AA254" s="3" t="s">
         <v>40</v>
@@ -19883,7 +19889,7 @@
         <v>253</v>
       </c>
       <c r="B255" s="7">
-        <v>2025092112</v>
+        <v>2025090797</v>
       </c>
       <c r="C255" s="7">
         <v>1</v>
@@ -19895,16 +19901,16 @@
         <v>610</v>
       </c>
       <c r="F255" s="7" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="G255" s="7" t="s">
-        <v>381</v>
+        <v>353</v>
       </c>
       <c r="H255" s="7" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="I255" s="7" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="J255" s="7"/>
       <c r="K255" s="7"/>
@@ -19912,10 +19918,10 @@
         <v>163</v>
       </c>
       <c r="M255" s="8" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="N255" s="8" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="O255" s="7" t="s">
         <v>39</v>
@@ -19949,7 +19955,7 @@
         <v>254</v>
       </c>
       <c r="B256" s="3">
-        <v>2025091544</v>
+        <v>2025092112</v>
       </c>
       <c r="C256" s="3">
         <v>1</v>
@@ -19961,31 +19967,27 @@
         <v>610</v>
       </c>
       <c r="F256" s="3" t="s">
-        <v>210</v>
+        <v>31</v>
       </c>
       <c r="G256" s="3" t="s">
-        <v>197</v>
+        <v>381</v>
       </c>
       <c r="H256" s="3" t="s">
-        <v>359</v>
+        <v>714</v>
       </c>
       <c r="I256" s="3" t="s">
-        <v>718</v>
-      </c>
-      <c r="J256" s="3" t="s">
-        <v>719</v>
-      </c>
-      <c r="K256" s="3" t="s">
-        <v>720</v>
-      </c>
+        <v>715</v>
+      </c>
+      <c r="J256" s="3"/>
+      <c r="K256" s="3"/>
       <c r="L256" s="6" t="s">
-        <v>721</v>
+        <v>163</v>
       </c>
       <c r="M256" s="6" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
       <c r="N256" s="6" t="s">
-        <v>723</v>
+        <v>717</v>
       </c>
       <c r="O256" s="3" t="s">
         <v>39</v>
@@ -19995,57 +19997,127 @@
       <c r="R256" s="3">
         <v>0</v>
       </c>
-      <c r="S256" s="3"/>
-      <c r="T256" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S256" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T256" s="3"/>
       <c r="U256" s="3"/>
       <c r="V256" s="3"/>
       <c r="W256" s="3"/>
       <c r="X256" s="3"/>
       <c r="Y256" s="3"/>
       <c r="Z256" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="AA256" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB256" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:28">
+      <c r="A257" s="7">
+        <v>255</v>
+      </c>
+      <c r="B257" s="7">
+        <v>2025091544</v>
+      </c>
+      <c r="C257" s="7">
+        <v>1</v>
+      </c>
+      <c r="D257" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E257" s="7" t="s">
+        <v>610</v>
+      </c>
+      <c r="F257" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="G257" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="H257" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="I257" s="7" t="s">
+        <v>718</v>
+      </c>
+      <c r="J257" s="7" t="s">
+        <v>719</v>
+      </c>
+      <c r="K257" s="7" t="s">
+        <v>720</v>
+      </c>
+      <c r="L257" s="8" t="s">
+        <v>721</v>
+      </c>
+      <c r="M257" s="8" t="s">
+        <v>722</v>
+      </c>
+      <c r="N257" s="8" t="s">
+        <v>723</v>
+      </c>
+      <c r="O257" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="P257" s="7"/>
+      <c r="Q257" s="7"/>
+      <c r="R257" s="7">
+        <v>0</v>
+      </c>
+      <c r="S257" s="7"/>
+      <c r="T257" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="U257" s="7"/>
+      <c r="V257" s="7"/>
+      <c r="W257" s="7"/>
+      <c r="X257" s="7"/>
+      <c r="Y257" s="7"/>
+      <c r="Z257" s="8" t="s">
         <v>724</v>
       </c>
-      <c r="AA256" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB256" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="257" spans="1:28">
-      <c r="A257" s="9"/>
-      <c r="B257" s="9"/>
-      <c r="C257" s="9"/>
-      <c r="D257" s="9"/>
-      <c r="E257" s="9"/>
-      <c r="F257" s="9"/>
-      <c r="G257" s="9"/>
-      <c r="H257" s="9"/>
-      <c r="I257" s="9"/>
-      <c r="J257" s="9"/>
-      <c r="K257" s="9"/>
-      <c r="L257" s="10"/>
-      <c r="M257" s="10"/>
-      <c r="N257" s="10"/>
-      <c r="O257" s="9"/>
-      <c r="P257" s="9"/>
-      <c r="Q257" s="9"/>
-      <c r="R257" s="9"/>
-      <c r="S257" s="9"/>
-      <c r="T257" s="9"/>
-      <c r="U257" s="9"/>
-      <c r="V257" s="9"/>
-      <c r="W257" s="9"/>
-      <c r="X257" s="9"/>
-      <c r="Y257" s="9"/>
-      <c r="Z257" s="10"/>
-      <c r="AA257" s="9" t="s">
+      <c r="AA257" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB257" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:28">
+      <c r="A258" s="9"/>
+      <c r="B258" s="9"/>
+      <c r="C258" s="9"/>
+      <c r="D258" s="9"/>
+      <c r="E258" s="9"/>
+      <c r="F258" s="9"/>
+      <c r="G258" s="9"/>
+      <c r="H258" s="9"/>
+      <c r="I258" s="9"/>
+      <c r="J258" s="9"/>
+      <c r="K258" s="9"/>
+      <c r="L258" s="10"/>
+      <c r="M258" s="10"/>
+      <c r="N258" s="10"/>
+      <c r="O258" s="9"/>
+      <c r="P258" s="9"/>
+      <c r="Q258" s="9"/>
+      <c r="R258" s="9"/>
+      <c r="S258" s="9"/>
+      <c r="T258" s="9"/>
+      <c r="U258" s="9"/>
+      <c r="V258" s="9"/>
+      <c r="W258" s="9"/>
+      <c r="X258" s="9"/>
+      <c r="Y258" s="9"/>
+      <c r="Z258" s="10"/>
+      <c r="AA258" s="9" t="s">
         <v>725</v>
       </c>
-      <c r="AB257" s="9">
-        <v>136</v>
+      <c r="AB258" s="9">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit - 09191736
</commit_message>
<xml_diff>
--- a/IM/202509_Service_Count_Report.xlsx
+++ b/IM/202509_Service_Count_Report.xlsx
@@ -2323,6 +2323,11 @@
     <t>北縣僑中三店</t>
   </si>
   <si>
+    <t>更換發票機
+換上 8155004438
+換下 8155006284</t>
+  </si>
+  <si>
     <t>15:25:00</t>
   </si>
   <si>
@@ -2332,11 +2337,6 @@
 1 嘗試交易 正常
 2 登出登入 正常
 3 重新開機 正常</t>
-  </si>
-  <si>
-    <t>更換發票機
-換上 8155004438
-換下 8155006284</t>
   </si>
   <si>
     <t>14:46:00</t>
@@ -3894,7 +3894,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="3">
-        <v>2025092220</v>
+        <v>2025092219</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -3933,7 +3933,7 @@
         <v>85</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P16" s="3"/>
       <c r="Q16" s="3">
@@ -3942,7 +3942,9 @@
       <c r="R16" s="3">
         <v>65895</v>
       </c>
-      <c r="S16" s="3"/>
+      <c r="S16" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
@@ -3964,7 +3966,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="7">
-        <v>2025092219</v>
+        <v>2025092220</v>
       </c>
       <c r="C17" s="7">
         <v>1</v>
@@ -4003,7 +4005,7 @@
         <v>85</v>
       </c>
       <c r="O17" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P17" s="7"/>
       <c r="Q17" s="7">
@@ -4012,9 +4014,7 @@
       <c r="R17" s="7">
         <v>65895</v>
       </c>
-      <c r="S17" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S17" s="7"/>
       <c r="T17" s="7"/>
       <c r="U17" s="7"/>
       <c r="V17" s="7"/>
@@ -9454,7 +9454,7 @@
         <v>96</v>
       </c>
       <c r="B98" s="3">
-        <v>2025091372</v>
+        <v>2025091374</v>
       </c>
       <c r="C98" s="3">
         <v>1</v>
@@ -9493,19 +9493,17 @@
         <v>380</v>
       </c>
       <c r="O98" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P98" s="3"/>
       <c r="Q98" s="3">
-        <v>29570</v>
+        <v>29573</v>
       </c>
       <c r="R98" s="3">
         <v>25842</v>
       </c>
       <c r="S98" s="3"/>
-      <c r="T98" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="T98" s="3"/>
       <c r="U98" s="3"/>
       <c r="V98" s="3"/>
       <c r="W98" s="3"/>
@@ -9526,7 +9524,7 @@
         <v>97</v>
       </c>
       <c r="B99" s="7">
-        <v>2025091373</v>
+        <v>2025091372</v>
       </c>
       <c r="C99" s="7">
         <v>1</v>
@@ -9569,15 +9567,15 @@
       </c>
       <c r="P99" s="7"/>
       <c r="Q99" s="7">
-        <v>29573</v>
+        <v>29570</v>
       </c>
       <c r="R99" s="7">
         <v>25842</v>
       </c>
-      <c r="S99" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="T99" s="7"/>
+      <c r="S99" s="7"/>
+      <c r="T99" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="U99" s="7"/>
       <c r="V99" s="7"/>
       <c r="W99" s="7"/>
@@ -9586,7 +9584,9 @@
       <c r="Z99" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="AA99" s="7"/>
+      <c r="AA99" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="AB99" s="7"/>
     </row>
     <row r="100" spans="1:28">
@@ -9594,7 +9594,7 @@
         <v>98</v>
       </c>
       <c r="B100" s="3">
-        <v>2025091374</v>
+        <v>2025091373</v>
       </c>
       <c r="C100" s="3">
         <v>1</v>
@@ -9633,7 +9633,7 @@
         <v>380</v>
       </c>
       <c r="O100" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P100" s="3"/>
       <c r="Q100" s="3">
@@ -9642,7 +9642,9 @@
       <c r="R100" s="3">
         <v>25842</v>
       </c>
-      <c r="S100" s="3"/>
+      <c r="S100" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T100" s="3"/>
       <c r="U100" s="3"/>
       <c r="V100" s="3"/>
@@ -9652,9 +9654,7 @@
       <c r="Z100" s="6" t="s">
         <v>382</v>
       </c>
-      <c r="AA100" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA100" s="3"/>
       <c r="AB100" s="3"/>
     </row>
     <row r="101" spans="1:28">
@@ -9934,7 +9934,7 @@
         <v>103</v>
       </c>
       <c r="B105" s="7">
-        <v>2025092238</v>
+        <v>2025092237</v>
       </c>
       <c r="C105" s="7">
         <v>1</v>
@@ -9973,7 +9973,7 @@
         <v>393</v>
       </c>
       <c r="O105" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P105" s="7"/>
       <c r="Q105" s="7">
@@ -9982,7 +9982,9 @@
       <c r="R105" s="7">
         <v>32582</v>
       </c>
-      <c r="S105" s="7"/>
+      <c r="S105" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T105" s="7"/>
       <c r="U105" s="7"/>
       <c r="V105" s="7"/>
@@ -9992,19 +9994,15 @@
       <c r="Z105" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="AA105" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB105" s="7">
-        <v>1</v>
-      </c>
+      <c r="AA105" s="7"/>
+      <c r="AB105" s="7"/>
     </row>
     <row r="106" spans="1:28">
       <c r="A106" s="3">
         <v>104</v>
       </c>
       <c r="B106" s="3">
-        <v>2025092237</v>
+        <v>2025092238</v>
       </c>
       <c r="C106" s="3">
         <v>1</v>
@@ -10043,7 +10041,7 @@
         <v>393</v>
       </c>
       <c r="O106" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P106" s="3"/>
       <c r="Q106" s="3">
@@ -10052,9 +10050,7 @@
       <c r="R106" s="3">
         <v>32582</v>
       </c>
-      <c r="S106" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S106" s="3"/>
       <c r="T106" s="3"/>
       <c r="U106" s="3"/>
       <c r="V106" s="3"/>
@@ -10064,7 +10060,9 @@
       <c r="Z106" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="AA106" s="3"/>
+      <c r="AA106" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="AB106" s="3"/>
     </row>
     <row r="107" spans="1:28">
@@ -10072,7 +10070,7 @@
         <v>105</v>
       </c>
       <c r="B107" s="7">
-        <v>2025090953</v>
+        <v>2025090954</v>
       </c>
       <c r="C107" s="7">
         <v>1</v>
@@ -10111,7 +10109,7 @@
         <v>397</v>
       </c>
       <c r="O107" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P107" s="7">
         <v>6429</v>
@@ -10122,9 +10120,7 @@
       <c r="R107" s="7">
         <v>18367</v>
       </c>
-      <c r="S107" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S107" s="7"/>
       <c r="T107" s="7"/>
       <c r="U107" s="7"/>
       <c r="V107" s="7"/>
@@ -10146,7 +10142,7 @@
         <v>106</v>
       </c>
       <c r="B108" s="3">
-        <v>2025090954</v>
+        <v>2025090953</v>
       </c>
       <c r="C108" s="3">
         <v>1</v>
@@ -10185,7 +10181,7 @@
         <v>397</v>
       </c>
       <c r="O108" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P108" s="3">
         <v>6429</v>
@@ -10196,7 +10192,9 @@
       <c r="R108" s="3">
         <v>18367</v>
       </c>
-      <c r="S108" s="3"/>
+      <c r="S108" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T108" s="3"/>
       <c r="U108" s="3"/>
       <c r="V108" s="3"/>
@@ -11256,7 +11254,7 @@
         <v>122</v>
       </c>
       <c r="B124" s="3">
-        <v>2025091707</v>
+        <v>2025091708</v>
       </c>
       <c r="C124" s="3">
         <v>1</v>
@@ -11295,16 +11293,14 @@
         <v>428</v>
       </c>
       <c r="O124" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P124" s="3"/>
       <c r="Q124" s="3"/>
       <c r="R124" s="3">
         <v>220600</v>
       </c>
-      <c r="S124" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S124" s="3"/>
       <c r="T124" s="3"/>
       <c r="U124" s="3"/>
       <c r="V124" s="3"/>
@@ -11314,15 +11310,19 @@
       <c r="Z124" s="6" t="s">
         <v>429</v>
       </c>
-      <c r="AA124" s="3"/>
-      <c r="AB124" s="3"/>
+      <c r="AA124" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB124" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="125" spans="1:28">
       <c r="A125" s="7">
         <v>123</v>
       </c>
       <c r="B125" s="7">
-        <v>2025091708</v>
+        <v>2025091707</v>
       </c>
       <c r="C125" s="7">
         <v>1</v>
@@ -11361,14 +11361,16 @@
         <v>428</v>
       </c>
       <c r="O125" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P125" s="7"/>
       <c r="Q125" s="7"/>
       <c r="R125" s="7">
         <v>220600</v>
       </c>
-      <c r="S125" s="7"/>
+      <c r="S125" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T125" s="7"/>
       <c r="U125" s="7"/>
       <c r="V125" s="7"/>
@@ -11378,9 +11380,7 @@
       <c r="Z125" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="AA125" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA125" s="7"/>
       <c r="AB125" s="7"/>
     </row>
     <row r="126" spans="1:28">
@@ -11932,7 +11932,7 @@
         <v>132</v>
       </c>
       <c r="B134" s="3">
-        <v>2025090971</v>
+        <v>2025090972</v>
       </c>
       <c r="C134" s="3">
         <v>1</v>
@@ -11969,16 +11969,14 @@
       </c>
       <c r="N134" s="6"/>
       <c r="O134" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P134" s="3"/>
       <c r="Q134" s="3"/>
       <c r="R134" s="3">
         <v>48000</v>
       </c>
-      <c r="S134" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S134" s="3"/>
       <c r="T134" s="3"/>
       <c r="U134" s="3"/>
       <c r="V134" s="3"/>
@@ -12000,7 +11998,7 @@
         <v>133</v>
       </c>
       <c r="B135" s="7">
-        <v>2025090972</v>
+        <v>2025090971</v>
       </c>
       <c r="C135" s="7">
         <v>1</v>
@@ -12037,14 +12035,16 @@
       </c>
       <c r="N135" s="8"/>
       <c r="O135" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P135" s="7"/>
       <c r="Q135" s="7"/>
       <c r="R135" s="7">
         <v>48000</v>
       </c>
-      <c r="S135" s="7"/>
+      <c r="S135" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T135" s="7"/>
       <c r="U135" s="7"/>
       <c r="V135" s="7"/>
@@ -13082,7 +13082,7 @@
         <v>149</v>
       </c>
       <c r="B151" s="7">
-        <v>2025092230</v>
+        <v>2025092229</v>
       </c>
       <c r="C151" s="7">
         <v>1</v>
@@ -13121,7 +13121,7 @@
         <v>483</v>
       </c>
       <c r="O151" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P151" s="7"/>
       <c r="Q151" s="7">
@@ -13130,7 +13130,9 @@
       <c r="R151" s="7">
         <v>22998</v>
       </c>
-      <c r="S151" s="7"/>
+      <c r="S151" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T151" s="7"/>
       <c r="U151" s="7"/>
       <c r="V151" s="7"/>
@@ -13140,19 +13142,15 @@
       <c r="Z151" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="AA151" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB151" s="7">
-        <v>1</v>
-      </c>
+      <c r="AA151" s="7"/>
+      <c r="AB151" s="7"/>
     </row>
     <row r="152" spans="1:28">
       <c r="A152" s="3">
         <v>150</v>
       </c>
       <c r="B152" s="3">
-        <v>2025092229</v>
+        <v>2025092230</v>
       </c>
       <c r="C152" s="3">
         <v>1</v>
@@ -13191,7 +13189,7 @@
         <v>483</v>
       </c>
       <c r="O152" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P152" s="3"/>
       <c r="Q152" s="3">
@@ -13200,9 +13198,7 @@
       <c r="R152" s="3">
         <v>22998</v>
       </c>
-      <c r="S152" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S152" s="3"/>
       <c r="T152" s="3"/>
       <c r="U152" s="3"/>
       <c r="V152" s="3"/>
@@ -13212,7 +13208,9 @@
       <c r="Z152" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="AA152" s="3"/>
+      <c r="AA152" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="AB152" s="3"/>
     </row>
     <row r="153" spans="1:28">
@@ -13758,7 +13756,7 @@
         <v>159</v>
       </c>
       <c r="B161" s="7">
-        <v>2025090402</v>
+        <v>2025090403</v>
       </c>
       <c r="C161" s="7">
         <v>1</v>
@@ -13797,16 +13795,14 @@
         <v>497</v>
       </c>
       <c r="O161" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P161" s="7"/>
       <c r="Q161" s="7"/>
       <c r="R161" s="7">
         <v>117282</v>
       </c>
-      <c r="S161" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S161" s="7"/>
       <c r="T161" s="7"/>
       <c r="U161" s="7"/>
       <c r="V161" s="7"/>
@@ -13816,15 +13812,19 @@
       <c r="Z161" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="AA161" s="7"/>
-      <c r="AB161" s="7"/>
+      <c r="AA161" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB161" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="162" spans="1:28">
       <c r="A162" s="3">
         <v>160</v>
       </c>
       <c r="B162" s="3">
-        <v>2025090403</v>
+        <v>2025090402</v>
       </c>
       <c r="C162" s="3">
         <v>1</v>
@@ -13863,14 +13863,16 @@
         <v>497</v>
       </c>
       <c r="O162" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P162" s="3"/>
       <c r="Q162" s="3"/>
       <c r="R162" s="3">
         <v>117282</v>
       </c>
-      <c r="S162" s="3"/>
+      <c r="S162" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T162" s="3"/>
       <c r="U162" s="3"/>
       <c r="V162" s="3"/>
@@ -13880,9 +13882,7 @@
       <c r="Z162" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="AA162" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA162" s="3"/>
       <c r="AB162" s="3"/>
     </row>
     <row r="163" spans="1:28">
@@ -20396,7 +20396,7 @@
         <v>258</v>
       </c>
       <c r="B260" s="3">
-        <v>2025090712</v>
+        <v>2025090821</v>
       </c>
       <c r="C260" s="3">
         <v>1</v>
@@ -20419,12 +20419,8 @@
       <c r="I260" s="3" t="s">
         <v>710</v>
       </c>
-      <c r="J260" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="K260" s="3" t="s">
-        <v>175</v>
-      </c>
+      <c r="J260" s="3"/>
+      <c r="K260" s="3"/>
       <c r="L260" s="6" t="s">
         <v>176</v>
       </c>
@@ -20435,36 +20431,36 @@
         <v>712</v>
       </c>
       <c r="O260" s="3" t="s">
-        <v>167</v>
+        <v>39</v>
       </c>
       <c r="P260" s="3"/>
       <c r="Q260" s="3"/>
       <c r="R260" s="3">
         <v>0</v>
       </c>
-      <c r="S260" s="3"/>
+      <c r="S260" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T260" s="3"/>
       <c r="U260" s="3"/>
       <c r="V260" s="3"/>
       <c r="W260" s="3"/>
       <c r="X260" s="3"/>
-      <c r="Y260" s="3"/>
+      <c r="Y260" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="Z260" s="6" t="s">
-        <v>713</v>
-      </c>
-      <c r="AA260" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB260" s="3">
-        <v>1</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="AA260" s="3"/>
+      <c r="AB260" s="3"/>
     </row>
     <row r="261" spans="1:28">
       <c r="A261" s="7">
         <v>259</v>
       </c>
       <c r="B261" s="7">
-        <v>2025090821</v>
+        <v>2025090712</v>
       </c>
       <c r="C261" s="7">
         <v>1</v>
@@ -20487,8 +20483,12 @@
       <c r="I261" s="7" t="s">
         <v>710</v>
       </c>
-      <c r="J261" s="7"/>
-      <c r="K261" s="7"/>
+      <c r="J261" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="K261" s="7" t="s">
+        <v>175</v>
+      </c>
       <c r="L261" s="8" t="s">
         <v>176</v>
       </c>
@@ -20499,28 +20499,26 @@
         <v>712</v>
       </c>
       <c r="O261" s="7" t="s">
-        <v>39</v>
+        <v>167</v>
       </c>
       <c r="P261" s="7"/>
       <c r="Q261" s="7"/>
       <c r="R261" s="7">
         <v>0</v>
       </c>
-      <c r="S261" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S261" s="7"/>
       <c r="T261" s="7"/>
       <c r="U261" s="7"/>
       <c r="V261" s="7"/>
       <c r="W261" s="7"/>
       <c r="X261" s="7"/>
-      <c r="Y261" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="Y261" s="7"/>
       <c r="Z261" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="AA261" s="7"/>
+        <v>713</v>
+      </c>
+      <c r="AA261" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="AB261" s="7"/>
     </row>
     <row r="262" spans="1:28">
@@ -21066,7 +21064,7 @@
         <v>268</v>
       </c>
       <c r="B270" s="3">
-        <v>2025091812</v>
+        <v>2025091612</v>
       </c>
       <c r="C270" s="3">
         <v>1</v>
@@ -21084,7 +21082,7 @@
         <v>686</v>
       </c>
       <c r="H270" s="3" t="s">
-        <v>743</v>
+        <v>344</v>
       </c>
       <c r="I270" s="3" t="s">
         <v>740</v>
@@ -21120,7 +21118,7 @@
       <c r="X270" s="3"/>
       <c r="Y270" s="3"/>
       <c r="Z270" s="6" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="AA270" s="3" t="s">
         <v>40</v>
@@ -21134,7 +21132,7 @@
         <v>269</v>
       </c>
       <c r="B271" s="7">
-        <v>2025091612</v>
+        <v>2025091812</v>
       </c>
       <c r="C271" s="7">
         <v>1</v>
@@ -21152,7 +21150,7 @@
         <v>686</v>
       </c>
       <c r="H271" s="7" t="s">
-        <v>344</v>
+        <v>744</v>
       </c>
       <c r="I271" s="7" t="s">
         <v>740</v>
@@ -21630,7 +21628,7 @@
         <v>770</v>
       </c>
       <c r="AB278" s="9">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>